<commit_message>
Change STDEV obsolate function to STDEV.S the new Excel build-in.
</commit_message>
<xml_diff>
--- a/01_Dimension 1-10/04_Internal Micrometer/04_Internal Micrometer 0-25 mm..xlsx
+++ b/01_Dimension 1-10/04_Internal Micrometer/04_Internal Micrometer 0-25 mm..xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pakaw\oxsoft\metrikos\proecho\01_Dimension 1-10\04_Internal Micrometer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pakaw\oxsoft\metrikos\evgenis\01_Dimension 1-10\04_Internal Micrometer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="435" windowWidth="27225" windowHeight="14775" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="435" windowWidth="27225" windowHeight="14775" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="11" r:id="rId1"/>
@@ -1885,7 +1885,7 @@
     <xf numFmtId="182" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="181" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="473">
+  <cellXfs count="469">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2760,204 +2760,6 @@
     <xf numFmtId="166" fontId="43" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="43" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="16" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2985,8 +2787,194 @@
     <xf numFmtId="178" fontId="49" fillId="0" borderId="11" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="43" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="55" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3011,21 +2999,6 @@
     </xf>
     <xf numFmtId="179" fontId="62" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3078,61 +3051,22 @@
     <xf numFmtId="177" fontId="17" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="11" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="14" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="11" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="8" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="9" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="17" fillId="0" borderId="12" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3144,13 +3078,13 @@
     <xf numFmtId="166" fontId="17" fillId="0" borderId="13" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="7" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="8" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="8" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="9" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="9" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="17" fillId="0" borderId="12" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3225,19 +3159,61 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="7" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="8" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="9" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="43" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="11" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="17" fillId="0" borderId="14" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="11" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3257,6 +3233,30 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3287,18 +3287,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="172" fontId="26" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3481,8 +3469,8 @@
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
@@ -5228,8 +5216,8 @@
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
@@ -5295,8 +5283,8 @@
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
@@ -39381,8 +39369,8 @@
   </sheetPr>
   <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16:W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="18.75" customHeight="1"/>
@@ -39833,30 +39821,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="22.5" customHeight="1">
-      <c r="A1" s="362" t="s">
+      <c r="A1" s="296" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="362"/>
-      <c r="C1" s="362"/>
-      <c r="D1" s="362"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="362"/>
-      <c r="G1" s="362"/>
-      <c r="H1" s="362"/>
-      <c r="I1" s="362"/>
-      <c r="J1" s="362"/>
+      <c r="B1" s="296"/>
+      <c r="C1" s="296"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
+      <c r="G1" s="296"/>
+      <c r="H1" s="296"/>
+      <c r="I1" s="296"/>
+      <c r="J1" s="296"/>
       <c r="K1" s="163" t="s">
         <v>61</v>
       </c>
       <c r="M1" s="163"/>
       <c r="N1" s="163"/>
-      <c r="O1" s="368" t="s">
+      <c r="O1" s="302" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="368"/>
-      <c r="Q1" s="368"/>
-      <c r="R1" s="368"/>
-      <c r="S1" s="368"/>
+      <c r="P1" s="302"/>
+      <c r="Q1" s="302"/>
+      <c r="R1" s="302"/>
+      <c r="S1" s="302"/>
       <c r="T1" s="164"/>
       <c r="U1" s="164"/>
       <c r="V1" s="164"/>
@@ -39880,41 +39868,41 @@
       <c r="AH1" s="170"/>
     </row>
     <row r="2" spans="1:41" ht="22.5" customHeight="1">
-      <c r="A2" s="362"/>
-      <c r="B2" s="362"/>
-      <c r="C2" s="362"/>
-      <c r="D2" s="362"/>
-      <c r="E2" s="362"/>
-      <c r="F2" s="362"/>
-      <c r="G2" s="362"/>
-      <c r="H2" s="362"/>
-      <c r="I2" s="362"/>
-      <c r="J2" s="362"/>
+      <c r="A2" s="296"/>
+      <c r="B2" s="296"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
       <c r="K2" s="164" t="s">
         <v>63</v>
       </c>
       <c r="M2" s="163"/>
       <c r="N2" s="164"/>
-      <c r="O2" s="369">
+      <c r="O2" s="303">
         <v>42370</v>
       </c>
-      <c r="P2" s="369"/>
-      <c r="Q2" s="369"/>
-      <c r="R2" s="369"/>
-      <c r="S2" s="369"/>
+      <c r="P2" s="303"/>
+      <c r="Q2" s="303"/>
+      <c r="R2" s="303"/>
+      <c r="S2" s="303"/>
       <c r="T2" s="164" t="s">
         <v>64</v>
       </c>
       <c r="V2" s="163"/>
       <c r="W2" s="167"/>
       <c r="X2" s="167"/>
-      <c r="Y2" s="370">
+      <c r="Y2" s="304">
         <v>42371</v>
       </c>
-      <c r="Z2" s="370"/>
-      <c r="AA2" s="370"/>
-      <c r="AB2" s="370"/>
-      <c r="AC2" s="370"/>
+      <c r="Z2" s="304"/>
+      <c r="AA2" s="304"/>
+      <c r="AB2" s="304"/>
+      <c r="AC2" s="304"/>
       <c r="AD2" s="167"/>
       <c r="AE2" s="165"/>
       <c r="AF2" s="165"/>
@@ -39923,18 +39911,18 @@
       <c r="AJ2" s="25"/>
     </row>
     <row r="3" spans="1:41" ht="22.5" customHeight="1">
-      <c r="A3" s="363" t="s">
+      <c r="A3" s="297" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="363"/>
-      <c r="C3" s="363"/>
-      <c r="D3" s="363"/>
-      <c r="E3" s="363"/>
-      <c r="F3" s="363"/>
-      <c r="G3" s="363"/>
-      <c r="H3" s="363"/>
-      <c r="I3" s="363"/>
-      <c r="J3" s="363"/>
+      <c r="B3" s="297"/>
+      <c r="C3" s="297"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="297"/>
+      <c r="I3" s="297"/>
+      <c r="J3" s="297"/>
       <c r="K3" s="163" t="s">
         <v>66</v>
       </c>
@@ -39964,18 +39952,18 @@
       <c r="AD3" s="163"/>
     </row>
     <row r="4" spans="1:41" ht="22.5" customHeight="1">
-      <c r="A4" s="364" t="s">
+      <c r="A4" s="298" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="364"/>
-      <c r="C4" s="364"/>
-      <c r="D4" s="364"/>
-      <c r="E4" s="364"/>
-      <c r="F4" s="364"/>
-      <c r="G4" s="364"/>
-      <c r="H4" s="364"/>
-      <c r="I4" s="364"/>
-      <c r="J4" s="364"/>
+      <c r="B4" s="298"/>
+      <c r="C4" s="298"/>
+      <c r="D4" s="298"/>
+      <c r="E4" s="298"/>
+      <c r="F4" s="298"/>
+      <c r="G4" s="298"/>
+      <c r="H4" s="298"/>
+      <c r="I4" s="298"/>
+      <c r="J4" s="298"/>
       <c r="K4" s="163" t="s">
         <v>54</v>
       </c>
@@ -40015,22 +40003,22 @@
       <c r="C5" s="158"/>
       <c r="D5" s="219"/>
       <c r="E5" s="219"/>
-      <c r="F5" s="345" t="s">
+      <c r="F5" s="305" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="345"/>
-      <c r="H5" s="345"/>
-      <c r="I5" s="345"/>
-      <c r="J5" s="345"/>
-      <c r="K5" s="345"/>
-      <c r="L5" s="345"/>
-      <c r="M5" s="345"/>
-      <c r="N5" s="345"/>
-      <c r="O5" s="345"/>
-      <c r="P5" s="345"/>
-      <c r="Q5" s="345"/>
-      <c r="R5" s="345"/>
-      <c r="S5" s="345"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="305"/>
+      <c r="K5" s="305"/>
+      <c r="L5" s="305"/>
+      <c r="M5" s="305"/>
+      <c r="N5" s="305"/>
+      <c r="O5" s="305"/>
+      <c r="P5" s="305"/>
+      <c r="Q5" s="305"/>
+      <c r="R5" s="305"/>
+      <c r="S5" s="305"/>
       <c r="T5" s="171"/>
       <c r="U5" s="171"/>
       <c r="V5" s="171"/>
@@ -40052,32 +40040,32 @@
       <c r="C6" s="158"/>
       <c r="D6" s="219"/>
       <c r="E6" s="219"/>
-      <c r="F6" s="365" t="s">
+      <c r="F6" s="299" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="365"/>
-      <c r="H6" s="365"/>
-      <c r="I6" s="365"/>
-      <c r="J6" s="365"/>
-      <c r="K6" s="365"/>
-      <c r="L6" s="365"/>
-      <c r="M6" s="365"/>
-      <c r="N6" s="365"/>
-      <c r="O6" s="365"/>
+      <c r="G6" s="299"/>
+      <c r="H6" s="299"/>
+      <c r="I6" s="299"/>
+      <c r="J6" s="299"/>
+      <c r="K6" s="299"/>
+      <c r="L6" s="299"/>
+      <c r="M6" s="299"/>
+      <c r="N6" s="299"/>
+      <c r="O6" s="299"/>
       <c r="P6" s="218" t="s">
         <v>72</v>
       </c>
       <c r="Q6" s="218"/>
       <c r="R6" s="220"/>
       <c r="S6" s="293"/>
-      <c r="T6" s="297" t="s">
+      <c r="T6" s="307" t="s">
         <v>84</v>
       </c>
-      <c r="U6" s="297"/>
-      <c r="V6" s="297"/>
-      <c r="W6" s="297"/>
-      <c r="X6" s="297"/>
-      <c r="Y6" s="297"/>
+      <c r="U6" s="307"/>
+      <c r="V6" s="307"/>
+      <c r="W6" s="307"/>
+      <c r="X6" s="307"/>
+      <c r="Y6" s="307"/>
       <c r="Z6" s="171"/>
       <c r="AA6" s="171"/>
       <c r="AB6" s="171"/>
@@ -40091,39 +40079,39 @@
       <c r="A7" s="171" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="371" t="s">
+      <c r="C7" s="306" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="371"/>
-      <c r="E7" s="371"/>
-      <c r="F7" s="371"/>
-      <c r="G7" s="371"/>
-      <c r="H7" s="371"/>
-      <c r="I7" s="371"/>
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="306"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="306"/>
       <c r="J7" s="172" t="s">
         <v>73</v>
       </c>
       <c r="K7" s="172"/>
       <c r="L7" s="172"/>
-      <c r="M7" s="371">
+      <c r="M7" s="306">
         <v>98778</v>
       </c>
-      <c r="N7" s="371"/>
-      <c r="O7" s="371"/>
-      <c r="P7" s="371"/>
-      <c r="Q7" s="371"/>
-      <c r="R7" s="371"/>
-      <c r="S7" s="366" t="s">
+      <c r="N7" s="306"/>
+      <c r="O7" s="306"/>
+      <c r="P7" s="306"/>
+      <c r="Q7" s="306"/>
+      <c r="R7" s="306"/>
+      <c r="S7" s="300" t="s">
         <v>57</v>
       </c>
-      <c r="T7" s="367"/>
-      <c r="U7" s="365" t="s">
+      <c r="T7" s="301"/>
+      <c r="U7" s="299" t="s">
         <v>86</v>
       </c>
-      <c r="V7" s="365"/>
-      <c r="W7" s="365"/>
-      <c r="X7" s="365"/>
-      <c r="Y7" s="365"/>
+      <c r="V7" s="299"/>
+      <c r="W7" s="299"/>
+      <c r="X7" s="299"/>
+      <c r="Y7" s="299"/>
       <c r="Z7" s="171"/>
       <c r="AA7" s="171"/>
       <c r="AB7" s="171"/>
@@ -40141,31 +40129,31 @@
       </c>
       <c r="B8" s="157"/>
       <c r="C8" s="158"/>
-      <c r="D8" s="297">
+      <c r="D8" s="307">
         <v>0</v>
       </c>
-      <c r="E8" s="297"/>
+      <c r="E8" s="307"/>
       <c r="F8" s="219" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="297">
+      <c r="G8" s="307">
         <v>25</v>
       </c>
-      <c r="H8" s="297"/>
+      <c r="H8" s="307"/>
       <c r="I8" s="175" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="220"/>
       <c r="K8" s="220"/>
-      <c r="L8" s="344" t="s">
+      <c r="L8" s="308" t="s">
         <v>76</v>
       </c>
-      <c r="M8" s="344"/>
-      <c r="N8" s="344"/>
-      <c r="O8" s="297">
+      <c r="M8" s="308"/>
+      <c r="N8" s="308"/>
+      <c r="O8" s="307">
         <v>1E-3</v>
       </c>
-      <c r="P8" s="297"/>
+      <c r="P8" s="307"/>
       <c r="Q8" s="171" t="s">
         <v>10</v>
       </c>
@@ -40207,21 +40195,21 @@
       </c>
       <c r="M9" s="220"/>
       <c r="N9" s="175"/>
-      <c r="O9" s="345"/>
-      <c r="P9" s="345"/>
-      <c r="Q9" s="345"/>
-      <c r="R9" s="345"/>
-      <c r="S9" s="345"/>
-      <c r="T9" s="345"/>
-      <c r="U9" s="345"/>
-      <c r="V9" s="345"/>
-      <c r="W9" s="345"/>
-      <c r="X9" s="345"/>
-      <c r="Y9" s="345"/>
-      <c r="Z9" s="345"/>
-      <c r="AA9" s="345"/>
-      <c r="AB9" s="345"/>
-      <c r="AC9" s="345"/>
+      <c r="O9" s="305"/>
+      <c r="P9" s="305"/>
+      <c r="Q9" s="305"/>
+      <c r="R9" s="305"/>
+      <c r="S9" s="305"/>
+      <c r="T9" s="305"/>
+      <c r="U9" s="305"/>
+      <c r="V9" s="305"/>
+      <c r="W9" s="305"/>
+      <c r="X9" s="305"/>
+      <c r="Y9" s="305"/>
+      <c r="Z9" s="305"/>
+      <c r="AA9" s="305"/>
+      <c r="AB9" s="305"/>
+      <c r="AC9" s="305"/>
       <c r="AD9" s="157"/>
       <c r="AE9" s="173"/>
       <c r="AF9" s="173"/>
@@ -40275,31 +40263,31 @@
       <c r="D11" s="174"/>
       <c r="E11" s="174"/>
       <c r="F11" s="174"/>
-      <c r="G11" s="346"/>
-      <c r="H11" s="346"/>
-      <c r="I11" s="346"/>
-      <c r="J11" s="346"/>
-      <c r="K11" s="346"/>
-      <c r="L11" s="346"/>
-      <c r="M11" s="346"/>
-      <c r="N11" s="346"/>
-      <c r="O11" s="346"/>
+      <c r="G11" s="309"/>
+      <c r="H11" s="309"/>
+      <c r="I11" s="309"/>
+      <c r="J11" s="309"/>
+      <c r="K11" s="309"/>
+      <c r="L11" s="309"/>
+      <c r="M11" s="309"/>
+      <c r="N11" s="309"/>
+      <c r="O11" s="309"/>
       <c r="P11" s="157"/>
       <c r="Q11" s="171"/>
       <c r="R11" s="176" t="s">
         <v>80</v>
       </c>
       <c r="S11" s="176"/>
-      <c r="T11" s="347"/>
-      <c r="U11" s="347"/>
-      <c r="V11" s="347"/>
-      <c r="W11" s="347"/>
-      <c r="X11" s="347"/>
-      <c r="Y11" s="347"/>
-      <c r="Z11" s="347"/>
-      <c r="AA11" s="347"/>
-      <c r="AB11" s="347"/>
-      <c r="AC11" s="347"/>
+      <c r="T11" s="310"/>
+      <c r="U11" s="310"/>
+      <c r="V11" s="310"/>
+      <c r="W11" s="310"/>
+      <c r="X11" s="310"/>
+      <c r="Y11" s="310"/>
+      <c r="Z11" s="310"/>
+      <c r="AA11" s="310"/>
+      <c r="AB11" s="310"/>
+      <c r="AC11" s="310"/>
       <c r="AD11" s="157"/>
       <c r="AE11" s="177"/>
       <c r="AF11" s="177"/>
@@ -40365,660 +40353,660 @@
     </row>
     <row r="14" spans="1:41" ht="21" customHeight="1">
       <c r="A14" s="159"/>
-      <c r="B14" s="358" t="s">
+      <c r="B14" s="329" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="339"/>
-      <c r="D14" s="339"/>
-      <c r="E14" s="329" t="s">
+      <c r="C14" s="330"/>
+      <c r="D14" s="330"/>
+      <c r="E14" s="314" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="330"/>
-      <c r="G14" s="330"/>
-      <c r="H14" s="330"/>
-      <c r="I14" s="330"/>
-      <c r="J14" s="330"/>
-      <c r="K14" s="330"/>
-      <c r="L14" s="330"/>
-      <c r="M14" s="330"/>
-      <c r="N14" s="330"/>
-      <c r="O14" s="330"/>
-      <c r="P14" s="331"/>
-      <c r="Q14" s="338" t="s">
+      <c r="F14" s="315"/>
+      <c r="G14" s="315"/>
+      <c r="H14" s="315"/>
+      <c r="I14" s="315"/>
+      <c r="J14" s="315"/>
+      <c r="K14" s="315"/>
+      <c r="L14" s="315"/>
+      <c r="M14" s="315"/>
+      <c r="N14" s="315"/>
+      <c r="O14" s="315"/>
+      <c r="P14" s="316"/>
+      <c r="Q14" s="355" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="339"/>
-      <c r="S14" s="340"/>
-      <c r="T14" s="332" t="s">
+      <c r="R14" s="330"/>
+      <c r="S14" s="356"/>
+      <c r="T14" s="349" t="s">
         <v>2</v>
       </c>
-      <c r="U14" s="333"/>
-      <c r="V14" s="333"/>
-      <c r="W14" s="334"/>
-      <c r="X14" s="350" t="s">
+      <c r="U14" s="350"/>
+      <c r="V14" s="350"/>
+      <c r="W14" s="351"/>
+      <c r="X14" s="317" t="s">
         <v>22</v>
       </c>
-      <c r="Y14" s="351"/>
-      <c r="Z14" s="352"/>
+      <c r="Y14" s="318"/>
+      <c r="Z14" s="319"/>
       <c r="AG14" s="159"/>
-      <c r="AH14" s="349"/>
-      <c r="AI14" s="349"/>
-      <c r="AJ14" s="349"/>
-      <c r="AK14" s="349"/>
+      <c r="AH14" s="313"/>
+      <c r="AI14" s="313"/>
+      <c r="AJ14" s="313"/>
+      <c r="AK14" s="313"/>
     </row>
     <row r="15" spans="1:41" ht="21" customHeight="1">
       <c r="A15" s="159"/>
-      <c r="B15" s="341"/>
-      <c r="C15" s="296"/>
-      <c r="D15" s="296"/>
-      <c r="E15" s="329" t="s">
+      <c r="B15" s="331"/>
+      <c r="C15" s="332"/>
+      <c r="D15" s="332"/>
+      <c r="E15" s="314" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="330"/>
-      <c r="G15" s="331"/>
-      <c r="H15" s="329" t="s">
+      <c r="F15" s="315"/>
+      <c r="G15" s="316"/>
+      <c r="H15" s="314" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="330"/>
-      <c r="J15" s="331"/>
-      <c r="K15" s="329" t="s">
+      <c r="I15" s="315"/>
+      <c r="J15" s="316"/>
+      <c r="K15" s="314" t="s">
         <v>98</v>
       </c>
-      <c r="L15" s="330"/>
-      <c r="M15" s="331"/>
-      <c r="N15" s="329" t="s">
+      <c r="L15" s="315"/>
+      <c r="M15" s="316"/>
+      <c r="N15" s="314" t="s">
         <v>99</v>
       </c>
-      <c r="O15" s="330"/>
-      <c r="P15" s="331"/>
-      <c r="Q15" s="341"/>
-      <c r="R15" s="296"/>
-      <c r="S15" s="342"/>
-      <c r="T15" s="335"/>
-      <c r="U15" s="336"/>
-      <c r="V15" s="336"/>
-      <c r="W15" s="337"/>
-      <c r="X15" s="353"/>
-      <c r="Y15" s="346"/>
-      <c r="Z15" s="354"/>
+      <c r="O15" s="315"/>
+      <c r="P15" s="316"/>
+      <c r="Q15" s="331"/>
+      <c r="R15" s="332"/>
+      <c r="S15" s="357"/>
+      <c r="T15" s="352"/>
+      <c r="U15" s="353"/>
+      <c r="V15" s="353"/>
+      <c r="W15" s="354"/>
+      <c r="X15" s="320"/>
+      <c r="Y15" s="309"/>
+      <c r="Z15" s="321"/>
       <c r="AG15" s="159"/>
-      <c r="AH15" s="348"/>
-      <c r="AI15" s="348"/>
+      <c r="AH15" s="312"/>
+      <c r="AI15" s="312"/>
       <c r="AJ15" s="180"/>
       <c r="AK15" s="180"/>
     </row>
     <row r="16" spans="1:41" ht="21" customHeight="1">
       <c r="A16" s="159"/>
-      <c r="B16" s="359">
+      <c r="B16" s="333">
         <v>0</v>
       </c>
-      <c r="C16" s="360"/>
-      <c r="D16" s="361"/>
-      <c r="E16" s="355">
+      <c r="C16" s="334"/>
+      <c r="D16" s="335"/>
+      <c r="E16" s="326">
         <v>0</v>
       </c>
-      <c r="F16" s="356"/>
-      <c r="G16" s="357"/>
-      <c r="H16" s="313">
+      <c r="F16" s="327"/>
+      <c r="G16" s="328"/>
+      <c r="H16" s="346">
         <v>0</v>
       </c>
-      <c r="I16" s="314"/>
-      <c r="J16" s="315"/>
-      <c r="K16" s="313">
+      <c r="I16" s="347"/>
+      <c r="J16" s="348"/>
+      <c r="K16" s="346">
         <v>0</v>
       </c>
-      <c r="L16" s="314"/>
-      <c r="M16" s="315"/>
-      <c r="N16" s="313">
+      <c r="L16" s="347"/>
+      <c r="M16" s="348"/>
+      <c r="N16" s="346">
         <v>1E-3</v>
       </c>
-      <c r="O16" s="314"/>
-      <c r="P16" s="315"/>
-      <c r="Q16" s="309">
+      <c r="O16" s="347"/>
+      <c r="P16" s="348"/>
+      <c r="Q16" s="365">
         <f>AVERAGE(E16:P16)</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="R16" s="310"/>
-      <c r="S16" s="311"/>
-      <c r="T16" s="302">
-        <f>STDEV(E16:P16)/SQRT(4)</f>
+      <c r="R16" s="366"/>
+      <c r="S16" s="367"/>
+      <c r="T16" s="362">
+        <f>_xlfn.STDEV.S(E16:P16)/SQRT(4)</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="U16" s="303"/>
-      <c r="V16" s="303"/>
-      <c r="W16" s="304"/>
-      <c r="X16" s="299">
+      <c r="U16" s="363"/>
+      <c r="V16" s="363"/>
+      <c r="W16" s="364"/>
+      <c r="X16" s="322">
         <f>Q16-B16</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="Y16" s="300"/>
-      <c r="Z16" s="301"/>
+      <c r="Y16" s="323"/>
+      <c r="Z16" s="324"/>
       <c r="AB16" s="295"/>
       <c r="AG16" s="159"/>
-      <c r="AH16" s="343"/>
-      <c r="AI16" s="343"/>
+      <c r="AH16" s="311"/>
+      <c r="AI16" s="311"/>
       <c r="AJ16" s="180"/>
       <c r="AK16" s="180"/>
     </row>
     <row r="17" spans="1:38" ht="21" customHeight="1">
       <c r="A17" s="159"/>
-      <c r="B17" s="323">
+      <c r="B17" s="336">
         <v>2.5</v>
       </c>
-      <c r="C17" s="323"/>
-      <c r="D17" s="323"/>
-      <c r="E17" s="316">
+      <c r="C17" s="336"/>
+      <c r="D17" s="336"/>
+      <c r="E17" s="325">
         <v>2.5</v>
       </c>
-      <c r="F17" s="316"/>
-      <c r="G17" s="316"/>
-      <c r="H17" s="316">
+      <c r="F17" s="325"/>
+      <c r="G17" s="325"/>
+      <c r="H17" s="325">
         <v>2.5019999999999998</v>
       </c>
-      <c r="I17" s="316"/>
-      <c r="J17" s="316"/>
-      <c r="K17" s="316">
+      <c r="I17" s="325"/>
+      <c r="J17" s="325"/>
+      <c r="K17" s="325">
         <v>2.5</v>
       </c>
-      <c r="L17" s="316"/>
-      <c r="M17" s="316"/>
-      <c r="N17" s="316">
+      <c r="L17" s="325"/>
+      <c r="M17" s="325"/>
+      <c r="N17" s="325">
         <v>2.5</v>
       </c>
-      <c r="O17" s="316"/>
-      <c r="P17" s="316"/>
-      <c r="Q17" s="312">
+      <c r="O17" s="325"/>
+      <c r="P17" s="325"/>
+      <c r="Q17" s="345">
         <f>AVERAGE(E17:P17)</f>
         <v>2.5004999999999997</v>
       </c>
-      <c r="R17" s="312"/>
-      <c r="S17" s="312"/>
-      <c r="T17" s="305">
-        <f t="shared" ref="T17:T26" si="0">STDEV(E17:P17)/SQRT(4)</f>
+      <c r="R17" s="345"/>
+      <c r="S17" s="345"/>
+      <c r="T17" s="362">
+        <f t="shared" ref="T17:T26" si="0">_xlfn.STDEV.S(E17:P17)/SQRT(4)</f>
         <v>4.9999999999994493E-4</v>
       </c>
-      <c r="U17" s="305"/>
-      <c r="V17" s="305"/>
-      <c r="W17" s="305"/>
-      <c r="X17" s="299">
+      <c r="U17" s="363"/>
+      <c r="V17" s="363"/>
+      <c r="W17" s="364"/>
+      <c r="X17" s="322">
         <f>Q17-B17</f>
         <v>4.9999999999972289E-4</v>
       </c>
-      <c r="Y17" s="300"/>
-      <c r="Z17" s="301"/>
-      <c r="AB17" s="298"/>
-      <c r="AC17" s="298"/>
+      <c r="Y17" s="323"/>
+      <c r="Z17" s="324"/>
+      <c r="AB17" s="361"/>
+      <c r="AC17" s="361"/>
       <c r="AG17" s="159"/>
-      <c r="AH17" s="343"/>
-      <c r="AI17" s="343"/>
+      <c r="AH17" s="311"/>
+      <c r="AI17" s="311"/>
       <c r="AJ17" s="180"/>
       <c r="AK17" s="180"/>
     </row>
     <row r="18" spans="1:38" ht="21" customHeight="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="323">
+      <c r="B18" s="336">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C18" s="323"/>
-      <c r="D18" s="323"/>
-      <c r="E18" s="316">
+      <c r="C18" s="336"/>
+      <c r="D18" s="336"/>
+      <c r="E18" s="325">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="316"/>
-      <c r="G18" s="316"/>
-      <c r="H18" s="316">
+      <c r="F18" s="325"/>
+      <c r="G18" s="325"/>
+      <c r="H18" s="325">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I18" s="316"/>
-      <c r="J18" s="316"/>
-      <c r="K18" s="316">
+      <c r="I18" s="325"/>
+      <c r="J18" s="325"/>
+      <c r="K18" s="325">
         <v>5.0999999999999996</v>
       </c>
-      <c r="L18" s="316"/>
-      <c r="M18" s="316"/>
-      <c r="N18" s="316">
+      <c r="L18" s="325"/>
+      <c r="M18" s="325"/>
+      <c r="N18" s="325">
         <v>5.0999999999999996</v>
       </c>
-      <c r="O18" s="316"/>
-      <c r="P18" s="316"/>
-      <c r="Q18" s="312">
+      <c r="O18" s="325"/>
+      <c r="P18" s="325"/>
+      <c r="Q18" s="345">
         <f t="shared" ref="Q18:Q26" si="1">AVERAGE(E18:P18)</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="R18" s="312"/>
-      <c r="S18" s="312"/>
-      <c r="T18" s="305">
+      <c r="R18" s="345"/>
+      <c r="S18" s="345"/>
+      <c r="T18" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U18" s="305"/>
-      <c r="V18" s="305"/>
-      <c r="W18" s="305"/>
-      <c r="X18" s="299">
+      <c r="U18" s="363"/>
+      <c r="V18" s="363"/>
+      <c r="W18" s="364"/>
+      <c r="X18" s="322">
         <f t="shared" ref="X18:X26" si="2">Q18-B18</f>
         <v>0</v>
       </c>
-      <c r="Y18" s="300"/>
-      <c r="Z18" s="301"/>
+      <c r="Y18" s="323"/>
+      <c r="Z18" s="324"/>
       <c r="AG18" s="159"/>
-      <c r="AH18" s="343"/>
-      <c r="AI18" s="343"/>
+      <c r="AH18" s="311"/>
+      <c r="AI18" s="311"/>
       <c r="AJ18" s="180"/>
       <c r="AK18" s="180"/>
     </row>
     <row r="19" spans="1:38" ht="21" customHeight="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="323">
+      <c r="B19" s="336">
         <v>7.7</v>
       </c>
-      <c r="C19" s="323"/>
-      <c r="D19" s="323"/>
-      <c r="E19" s="316">
+      <c r="C19" s="336"/>
+      <c r="D19" s="336"/>
+      <c r="E19" s="325">
         <v>7.7</v>
       </c>
-      <c r="F19" s="316"/>
-      <c r="G19" s="316"/>
-      <c r="H19" s="316">
+      <c r="F19" s="325"/>
+      <c r="G19" s="325"/>
+      <c r="H19" s="325">
         <v>7.7</v>
       </c>
-      <c r="I19" s="316"/>
-      <c r="J19" s="316"/>
-      <c r="K19" s="316">
+      <c r="I19" s="325"/>
+      <c r="J19" s="325"/>
+      <c r="K19" s="325">
         <v>7.7</v>
       </c>
-      <c r="L19" s="316"/>
-      <c r="M19" s="316"/>
-      <c r="N19" s="316">
+      <c r="L19" s="325"/>
+      <c r="M19" s="325"/>
+      <c r="N19" s="325">
         <v>7.7</v>
       </c>
-      <c r="O19" s="316"/>
-      <c r="P19" s="316"/>
-      <c r="Q19" s="312">
+      <c r="O19" s="325"/>
+      <c r="P19" s="325"/>
+      <c r="Q19" s="345">
         <f t="shared" si="1"/>
         <v>7.7</v>
       </c>
-      <c r="R19" s="312"/>
-      <c r="S19" s="312"/>
-      <c r="T19" s="305">
+      <c r="R19" s="345"/>
+      <c r="S19" s="345"/>
+      <c r="T19" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="305"/>
-      <c r="V19" s="305"/>
-      <c r="W19" s="305"/>
-      <c r="X19" s="299">
+      <c r="U19" s="363"/>
+      <c r="V19" s="363"/>
+      <c r="W19" s="364"/>
+      <c r="X19" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="300"/>
-      <c r="Z19" s="301"/>
+      <c r="Y19" s="323"/>
+      <c r="Z19" s="324"/>
       <c r="AG19" s="159"/>
-      <c r="AH19" s="343"/>
-      <c r="AI19" s="343"/>
+      <c r="AH19" s="311"/>
+      <c r="AI19" s="311"/>
       <c r="AJ19" s="180"/>
       <c r="AK19" s="180"/>
     </row>
     <row r="20" spans="1:38" ht="21" customHeight="1">
       <c r="A20" s="159"/>
-      <c r="B20" s="323">
+      <c r="B20" s="336">
         <v>10.3</v>
       </c>
-      <c r="C20" s="323"/>
-      <c r="D20" s="323"/>
-      <c r="E20" s="316">
+      <c r="C20" s="336"/>
+      <c r="D20" s="336"/>
+      <c r="E20" s="325">
         <v>10.3</v>
       </c>
-      <c r="F20" s="316"/>
-      <c r="G20" s="316"/>
-      <c r="H20" s="316">
+      <c r="F20" s="325"/>
+      <c r="G20" s="325"/>
+      <c r="H20" s="325">
         <v>10.3</v>
       </c>
-      <c r="I20" s="316"/>
-      <c r="J20" s="316"/>
-      <c r="K20" s="316">
+      <c r="I20" s="325"/>
+      <c r="J20" s="325"/>
+      <c r="K20" s="325">
         <v>10.3</v>
       </c>
-      <c r="L20" s="316"/>
-      <c r="M20" s="316"/>
-      <c r="N20" s="316">
+      <c r="L20" s="325"/>
+      <c r="M20" s="325"/>
+      <c r="N20" s="325">
         <v>10.3</v>
       </c>
-      <c r="O20" s="316"/>
-      <c r="P20" s="316"/>
-      <c r="Q20" s="312">
+      <c r="O20" s="325"/>
+      <c r="P20" s="325"/>
+      <c r="Q20" s="345">
         <f t="shared" si="1"/>
         <v>10.3</v>
       </c>
-      <c r="R20" s="312"/>
-      <c r="S20" s="312"/>
-      <c r="T20" s="305">
+      <c r="R20" s="345"/>
+      <c r="S20" s="345"/>
+      <c r="T20" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U20" s="305"/>
-      <c r="V20" s="305"/>
-      <c r="W20" s="305"/>
-      <c r="X20" s="299">
+      <c r="U20" s="363"/>
+      <c r="V20" s="363"/>
+      <c r="W20" s="364"/>
+      <c r="X20" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="300"/>
-      <c r="Z20" s="301"/>
+      <c r="Y20" s="323"/>
+      <c r="Z20" s="324"/>
       <c r="AG20" s="159"/>
-      <c r="AH20" s="343"/>
-      <c r="AI20" s="343"/>
+      <c r="AH20" s="311"/>
+      <c r="AI20" s="311"/>
       <c r="AJ20" s="180"/>
       <c r="AK20" s="180"/>
     </row>
     <row r="21" spans="1:38" ht="21" customHeight="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="323">
+      <c r="B21" s="336">
         <v>12.9</v>
       </c>
-      <c r="C21" s="323"/>
-      <c r="D21" s="323"/>
-      <c r="E21" s="316">
+      <c r="C21" s="336"/>
+      <c r="D21" s="336"/>
+      <c r="E21" s="325">
         <v>12.9</v>
       </c>
-      <c r="F21" s="316"/>
-      <c r="G21" s="316"/>
-      <c r="H21" s="316">
+      <c r="F21" s="325"/>
+      <c r="G21" s="325"/>
+      <c r="H21" s="325">
         <v>12.9</v>
       </c>
-      <c r="I21" s="316"/>
-      <c r="J21" s="316"/>
-      <c r="K21" s="316">
+      <c r="I21" s="325"/>
+      <c r="J21" s="325"/>
+      <c r="K21" s="325">
         <v>12.9</v>
       </c>
-      <c r="L21" s="316"/>
-      <c r="M21" s="316"/>
-      <c r="N21" s="316">
+      <c r="L21" s="325"/>
+      <c r="M21" s="325"/>
+      <c r="N21" s="325">
         <v>12.9</v>
       </c>
-      <c r="O21" s="316"/>
-      <c r="P21" s="316"/>
-      <c r="Q21" s="312">
+      <c r="O21" s="325"/>
+      <c r="P21" s="325"/>
+      <c r="Q21" s="345">
         <f t="shared" si="1"/>
         <v>12.9</v>
       </c>
-      <c r="R21" s="312"/>
-      <c r="S21" s="312"/>
-      <c r="T21" s="305">
+      <c r="R21" s="345"/>
+      <c r="S21" s="345"/>
+      <c r="T21" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U21" s="305"/>
-      <c r="V21" s="305"/>
-      <c r="W21" s="305"/>
-      <c r="X21" s="299">
+      <c r="U21" s="363"/>
+      <c r="V21" s="363"/>
+      <c r="W21" s="364"/>
+      <c r="X21" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y21" s="300"/>
-      <c r="Z21" s="301"/>
+      <c r="Y21" s="323"/>
+      <c r="Z21" s="324"/>
       <c r="AG21" s="159"/>
-      <c r="AH21" s="343"/>
-      <c r="AI21" s="343"/>
+      <c r="AH21" s="311"/>
+      <c r="AI21" s="311"/>
       <c r="AJ21" s="180"/>
       <c r="AK21" s="180"/>
     </row>
     <row r="22" spans="1:38" ht="21" customHeight="1">
       <c r="A22" s="159"/>
-      <c r="B22" s="323">
+      <c r="B22" s="336">
         <v>15</v>
       </c>
-      <c r="C22" s="323"/>
-      <c r="D22" s="323"/>
-      <c r="E22" s="316">
+      <c r="C22" s="336"/>
+      <c r="D22" s="336"/>
+      <c r="E22" s="325">
         <v>15</v>
       </c>
-      <c r="F22" s="316"/>
-      <c r="G22" s="316"/>
-      <c r="H22" s="316">
+      <c r="F22" s="325"/>
+      <c r="G22" s="325"/>
+      <c r="H22" s="325">
         <v>15</v>
       </c>
-      <c r="I22" s="316"/>
-      <c r="J22" s="316"/>
-      <c r="K22" s="316">
+      <c r="I22" s="325"/>
+      <c r="J22" s="325"/>
+      <c r="K22" s="325">
         <v>15</v>
       </c>
-      <c r="L22" s="316"/>
-      <c r="M22" s="316"/>
-      <c r="N22" s="316">
+      <c r="L22" s="325"/>
+      <c r="M22" s="325"/>
+      <c r="N22" s="325">
         <v>15</v>
       </c>
-      <c r="O22" s="316"/>
-      <c r="P22" s="316"/>
-      <c r="Q22" s="312">
+      <c r="O22" s="325"/>
+      <c r="P22" s="325"/>
+      <c r="Q22" s="345">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R22" s="312"/>
-      <c r="S22" s="312"/>
-      <c r="T22" s="305">
+      <c r="R22" s="345"/>
+      <c r="S22" s="345"/>
+      <c r="T22" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U22" s="305"/>
-      <c r="V22" s="305"/>
-      <c r="W22" s="305"/>
-      <c r="X22" s="299">
+      <c r="U22" s="363"/>
+      <c r="V22" s="363"/>
+      <c r="W22" s="364"/>
+      <c r="X22" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="300"/>
-      <c r="Z22" s="301"/>
+      <c r="Y22" s="323"/>
+      <c r="Z22" s="324"/>
       <c r="AG22" s="159"/>
-      <c r="AH22" s="343"/>
-      <c r="AI22" s="343"/>
+      <c r="AH22" s="311"/>
+      <c r="AI22" s="311"/>
       <c r="AJ22" s="180"/>
       <c r="AK22" s="180"/>
     </row>
     <row r="23" spans="1:38" ht="21" customHeight="1">
       <c r="A23" s="159"/>
-      <c r="B23" s="323">
+      <c r="B23" s="336">
         <v>17.600000000000001</v>
       </c>
-      <c r="C23" s="323"/>
-      <c r="D23" s="323"/>
-      <c r="E23" s="316">
+      <c r="C23" s="336"/>
+      <c r="D23" s="336"/>
+      <c r="E23" s="325">
         <v>17.600000000000001</v>
       </c>
-      <c r="F23" s="316"/>
-      <c r="G23" s="316"/>
-      <c r="H23" s="316">
+      <c r="F23" s="325"/>
+      <c r="G23" s="325"/>
+      <c r="H23" s="325">
         <v>17.600000000000001</v>
       </c>
-      <c r="I23" s="316"/>
-      <c r="J23" s="316"/>
-      <c r="K23" s="316">
+      <c r="I23" s="325"/>
+      <c r="J23" s="325"/>
+      <c r="K23" s="325">
         <v>17.600000000000001</v>
       </c>
-      <c r="L23" s="316"/>
-      <c r="M23" s="316"/>
-      <c r="N23" s="316">
+      <c r="L23" s="325"/>
+      <c r="M23" s="325"/>
+      <c r="N23" s="325">
         <v>17.600000000000001</v>
       </c>
-      <c r="O23" s="316"/>
-      <c r="P23" s="316"/>
-      <c r="Q23" s="312">
+      <c r="O23" s="325"/>
+      <c r="P23" s="325"/>
+      <c r="Q23" s="345">
         <f t="shared" si="1"/>
         <v>17.600000000000001</v>
       </c>
-      <c r="R23" s="312"/>
-      <c r="S23" s="312"/>
-      <c r="T23" s="305">
+      <c r="R23" s="345"/>
+      <c r="S23" s="345"/>
+      <c r="T23" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U23" s="305"/>
-      <c r="V23" s="305"/>
-      <c r="W23" s="305"/>
-      <c r="X23" s="299">
+      <c r="U23" s="363"/>
+      <c r="V23" s="363"/>
+      <c r="W23" s="364"/>
+      <c r="X23" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y23" s="300"/>
-      <c r="Z23" s="301"/>
+      <c r="Y23" s="323"/>
+      <c r="Z23" s="324"/>
       <c r="AG23" s="159"/>
-      <c r="AH23" s="343"/>
-      <c r="AI23" s="343"/>
+      <c r="AH23" s="311"/>
+      <c r="AI23" s="311"/>
       <c r="AJ23" s="180"/>
       <c r="AK23" s="180"/>
     </row>
     <row r="24" spans="1:38" ht="21" customHeight="1">
       <c r="A24" s="159"/>
-      <c r="B24" s="323">
+      <c r="B24" s="336">
         <v>20.2</v>
       </c>
-      <c r="C24" s="323"/>
-      <c r="D24" s="323"/>
-      <c r="E24" s="316">
+      <c r="C24" s="336"/>
+      <c r="D24" s="336"/>
+      <c r="E24" s="325">
         <v>20.2</v>
       </c>
-      <c r="F24" s="316"/>
-      <c r="G24" s="316"/>
-      <c r="H24" s="316">
+      <c r="F24" s="325"/>
+      <c r="G24" s="325"/>
+      <c r="H24" s="325">
         <v>20.2</v>
       </c>
-      <c r="I24" s="316"/>
-      <c r="J24" s="316"/>
-      <c r="K24" s="316">
+      <c r="I24" s="325"/>
+      <c r="J24" s="325"/>
+      <c r="K24" s="325">
         <v>20.2</v>
       </c>
-      <c r="L24" s="316"/>
-      <c r="M24" s="316"/>
-      <c r="N24" s="316">
+      <c r="L24" s="325"/>
+      <c r="M24" s="325"/>
+      <c r="N24" s="325">
         <v>20.2</v>
       </c>
-      <c r="O24" s="316"/>
-      <c r="P24" s="316"/>
-      <c r="Q24" s="312">
+      <c r="O24" s="325"/>
+      <c r="P24" s="325"/>
+      <c r="Q24" s="345">
         <f t="shared" si="1"/>
         <v>20.2</v>
       </c>
-      <c r="R24" s="312"/>
-      <c r="S24" s="312"/>
-      <c r="T24" s="305">
+      <c r="R24" s="345"/>
+      <c r="S24" s="345"/>
+      <c r="T24" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U24" s="305"/>
-      <c r="V24" s="305"/>
-      <c r="W24" s="305"/>
-      <c r="X24" s="299">
+      <c r="U24" s="363"/>
+      <c r="V24" s="363"/>
+      <c r="W24" s="364"/>
+      <c r="X24" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y24" s="300"/>
-      <c r="Z24" s="301"/>
+      <c r="Y24" s="323"/>
+      <c r="Z24" s="324"/>
       <c r="AG24" s="159"/>
-      <c r="AH24" s="343"/>
-      <c r="AI24" s="343"/>
+      <c r="AH24" s="311"/>
+      <c r="AI24" s="311"/>
       <c r="AJ24" s="180"/>
       <c r="AK24" s="180"/>
     </row>
     <row r="25" spans="1:38" ht="21" customHeight="1">
       <c r="A25" s="159"/>
-      <c r="B25" s="323">
+      <c r="B25" s="336">
         <v>22.8</v>
       </c>
-      <c r="C25" s="323"/>
-      <c r="D25" s="323"/>
-      <c r="E25" s="316">
+      <c r="C25" s="336"/>
+      <c r="D25" s="336"/>
+      <c r="E25" s="325">
         <v>22.8</v>
       </c>
-      <c r="F25" s="316"/>
-      <c r="G25" s="316"/>
-      <c r="H25" s="316">
+      <c r="F25" s="325"/>
+      <c r="G25" s="325"/>
+      <c r="H25" s="325">
         <v>22.8</v>
       </c>
-      <c r="I25" s="316"/>
-      <c r="J25" s="316"/>
-      <c r="K25" s="316">
+      <c r="I25" s="325"/>
+      <c r="J25" s="325"/>
+      <c r="K25" s="325">
         <v>22.8</v>
       </c>
-      <c r="L25" s="316"/>
-      <c r="M25" s="316"/>
-      <c r="N25" s="316">
+      <c r="L25" s="325"/>
+      <c r="M25" s="325"/>
+      <c r="N25" s="325">
         <v>22.8</v>
       </c>
-      <c r="O25" s="316"/>
-      <c r="P25" s="316"/>
-      <c r="Q25" s="312">
+      <c r="O25" s="325"/>
+      <c r="P25" s="325"/>
+      <c r="Q25" s="345">
         <f t="shared" si="1"/>
         <v>22.8</v>
       </c>
-      <c r="R25" s="312"/>
-      <c r="S25" s="312"/>
-      <c r="T25" s="305">
+      <c r="R25" s="345"/>
+      <c r="S25" s="345"/>
+      <c r="T25" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U25" s="305"/>
-      <c r="V25" s="305"/>
-      <c r="W25" s="305"/>
-      <c r="X25" s="299">
+      <c r="U25" s="363"/>
+      <c r="V25" s="363"/>
+      <c r="W25" s="364"/>
+      <c r="X25" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y25" s="300"/>
-      <c r="Z25" s="301"/>
+      <c r="Y25" s="323"/>
+      <c r="Z25" s="324"/>
       <c r="AG25" s="159"/>
-      <c r="AH25" s="343"/>
-      <c r="AI25" s="343"/>
+      <c r="AH25" s="311"/>
+      <c r="AI25" s="311"/>
       <c r="AJ25" s="180"/>
       <c r="AK25" s="180"/>
     </row>
     <row r="26" spans="1:38" ht="21" customHeight="1">
       <c r="A26" s="159"/>
-      <c r="B26" s="320">
+      <c r="B26" s="358">
         <v>25</v>
       </c>
-      <c r="C26" s="321"/>
-      <c r="D26" s="322"/>
-      <c r="E26" s="317">
+      <c r="C26" s="359"/>
+      <c r="D26" s="360"/>
+      <c r="E26" s="337">
         <v>25</v>
       </c>
-      <c r="F26" s="318"/>
-      <c r="G26" s="319"/>
-      <c r="H26" s="317">
+      <c r="F26" s="338"/>
+      <c r="G26" s="339"/>
+      <c r="H26" s="337">
         <v>25</v>
       </c>
-      <c r="I26" s="318"/>
-      <c r="J26" s="319"/>
-      <c r="K26" s="317">
+      <c r="I26" s="338"/>
+      <c r="J26" s="339"/>
+      <c r="K26" s="337">
         <v>25</v>
       </c>
-      <c r="L26" s="318"/>
-      <c r="M26" s="319"/>
-      <c r="N26" s="317">
+      <c r="L26" s="338"/>
+      <c r="M26" s="339"/>
+      <c r="N26" s="337">
         <v>25</v>
       </c>
-      <c r="O26" s="318"/>
-      <c r="P26" s="319"/>
-      <c r="Q26" s="326">
+      <c r="O26" s="338"/>
+      <c r="P26" s="339"/>
+      <c r="Q26" s="342">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="R26" s="327"/>
-      <c r="S26" s="328"/>
-      <c r="T26" s="306">
+      <c r="R26" s="343"/>
+      <c r="S26" s="344"/>
+      <c r="T26" s="362">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U26" s="307"/>
-      <c r="V26" s="307"/>
-      <c r="W26" s="308"/>
-      <c r="X26" s="299">
+      <c r="U26" s="363"/>
+      <c r="V26" s="363"/>
+      <c r="W26" s="364"/>
+      <c r="X26" s="322">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y26" s="300"/>
-      <c r="Z26" s="301"/>
+      <c r="Y26" s="323"/>
+      <c r="Z26" s="324"/>
       <c r="AG26" s="159"/>
-      <c r="AH26" s="343"/>
-      <c r="AI26" s="343"/>
+      <c r="AH26" s="311"/>
+      <c r="AI26" s="311"/>
       <c r="AJ26" s="180"/>
       <c r="AK26" s="180"/>
     </row>
@@ -41029,22 +41017,22 @@
       <c r="E27" s="190"/>
       <c r="F27" s="191"/>
       <c r="G27" s="191"/>
-      <c r="H27" s="324"/>
-      <c r="I27" s="324"/>
-      <c r="J27" s="324"/>
-      <c r="K27" s="324"/>
-      <c r="L27" s="324"/>
-      <c r="M27" s="324"/>
-      <c r="N27" s="324"/>
-      <c r="O27" s="324"/>
-      <c r="P27" s="324"/>
-      <c r="Q27" s="324"/>
-      <c r="R27" s="324"/>
-      <c r="S27" s="324"/>
-      <c r="T27" s="324"/>
-      <c r="U27" s="324"/>
-      <c r="V27" s="324"/>
-      <c r="W27" s="325"/>
+      <c r="H27" s="340"/>
+      <c r="I27" s="340"/>
+      <c r="J27" s="340"/>
+      <c r="K27" s="340"/>
+      <c r="L27" s="340"/>
+      <c r="M27" s="340"/>
+      <c r="N27" s="340"/>
+      <c r="O27" s="340"/>
+      <c r="P27" s="340"/>
+      <c r="Q27" s="340"/>
+      <c r="R27" s="340"/>
+      <c r="S27" s="340"/>
+      <c r="T27" s="340"/>
+      <c r="U27" s="340"/>
+      <c r="V27" s="340"/>
+      <c r="W27" s="341"/>
       <c r="X27" s="184"/>
       <c r="Y27" s="184"/>
       <c r="Z27" s="184"/>
@@ -41108,16 +41096,16 @@
       <c r="C29" s="155"/>
       <c r="D29" s="155"/>
       <c r="E29" s="155"/>
-      <c r="F29" s="296" t="s">
+      <c r="F29" s="332" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="296"/>
-      <c r="H29" s="296"/>
-      <c r="I29" s="296"/>
-      <c r="J29" s="296"/>
-      <c r="K29" s="296"/>
-      <c r="L29" s="296"/>
-      <c r="M29" s="296"/>
+      <c r="G29" s="332"/>
+      <c r="H29" s="332"/>
+      <c r="I29" s="332"/>
+      <c r="J29" s="332"/>
+      <c r="K29" s="332"/>
+      <c r="L29" s="332"/>
+      <c r="M29" s="332"/>
       <c r="N29" s="222"/>
     </row>
     <row r="30" spans="1:38" ht="20.100000000000001" customHeight="1">
@@ -41155,18 +41143,108 @@
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="F6:O6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="F5:S5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="M7:R7"/>
-    <mergeCell ref="U7:Y7"/>
+    <mergeCell ref="F29:M29"/>
+    <mergeCell ref="T6:Y6"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="X22:Z22"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="X20:Z20"/>
+    <mergeCell ref="X19:Z19"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="T26:W26"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="T14:W15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="Q14:S15"/>
+    <mergeCell ref="E14:P14"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="AH26:AI26"/>
+    <mergeCell ref="AH24:AI24"/>
+    <mergeCell ref="AH25:AI25"/>
+    <mergeCell ref="AH21:AI21"/>
+    <mergeCell ref="AH23:AI23"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AH20:AI20"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="X25:Z25"/>
+    <mergeCell ref="X26:Z26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="T21:W21"/>
+    <mergeCell ref="T22:W22"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="T25:W25"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="L8:N8"/>
@@ -41191,108 +41269,18 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="T18:W18"/>
     <mergeCell ref="T19:W19"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="AH26:AI26"/>
-    <mergeCell ref="AH24:AI24"/>
-    <mergeCell ref="AH25:AI25"/>
-    <mergeCell ref="AH21:AI21"/>
-    <mergeCell ref="AH23:AI23"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AH20:AI20"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="X25:Z25"/>
-    <mergeCell ref="X26:Z26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="T20:W20"/>
-    <mergeCell ref="T21:W21"/>
-    <mergeCell ref="T22:W22"/>
-    <mergeCell ref="T23:W23"/>
-    <mergeCell ref="T24:W24"/>
-    <mergeCell ref="T25:W25"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="T14:W15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="Q14:S15"/>
-    <mergeCell ref="E14:P14"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="F29:M29"/>
-    <mergeCell ref="T6:Y6"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="X22:Z22"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="X20:Z20"/>
-    <mergeCell ref="X19:Z19"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="T16:W16"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="T26:W26"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="F6:O6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="F5:S5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="M7:R7"/>
+    <mergeCell ref="U7:Y7"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.74803149606299213" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="97" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -41928,32 +41916,32 @@
     <row r="1" spans="1:27" ht="13.5" customHeight="1"/>
     <row r="2" spans="1:27" ht="14.1" customHeight="1"/>
     <row r="3" spans="1:27" ht="35.450000000000003" customHeight="1">
-      <c r="A3" s="375" t="s">
+      <c r="A3" s="371" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="375"/>
-      <c r="C3" s="375"/>
-      <c r="D3" s="375"/>
-      <c r="E3" s="375"/>
-      <c r="F3" s="375"/>
-      <c r="G3" s="375"/>
-      <c r="H3" s="375"/>
-      <c r="I3" s="375"/>
-      <c r="J3" s="375"/>
-      <c r="K3" s="375"/>
-      <c r="L3" s="375"/>
-      <c r="M3" s="375"/>
-      <c r="N3" s="375"/>
-      <c r="O3" s="375"/>
-      <c r="P3" s="375"/>
-      <c r="Q3" s="375"/>
-      <c r="R3" s="375"/>
-      <c r="S3" s="375"/>
-      <c r="T3" s="375"/>
-      <c r="U3" s="375"/>
-      <c r="V3" s="375"/>
-      <c r="W3" s="375"/>
-      <c r="X3" s="375"/>
+      <c r="B3" s="371"/>
+      <c r="C3" s="371"/>
+      <c r="D3" s="371"/>
+      <c r="E3" s="371"/>
+      <c r="F3" s="371"/>
+      <c r="G3" s="371"/>
+      <c r="H3" s="371"/>
+      <c r="I3" s="371"/>
+      <c r="J3" s="371"/>
+      <c r="K3" s="371"/>
+      <c r="L3" s="371"/>
+      <c r="M3" s="371"/>
+      <c r="N3" s="371"/>
+      <c r="O3" s="371"/>
+      <c r="P3" s="371"/>
+      <c r="Q3" s="371"/>
+      <c r="R3" s="371"/>
+      <c r="S3" s="371"/>
+      <c r="T3" s="371"/>
+      <c r="U3" s="371"/>
+      <c r="V3" s="371"/>
+      <c r="W3" s="371"/>
+      <c r="X3" s="371"/>
     </row>
     <row r="4" spans="1:27" s="83" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="82"/>
@@ -42302,12 +42290,12 @@
       <c r="I15" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="376">
+      <c r="J15" s="372">
         <f>Data!M7</f>
         <v>98778</v>
       </c>
-      <c r="K15" s="376"/>
-      <c r="L15" s="376"/>
+      <c r="K15" s="372"/>
+      <c r="L15" s="372"/>
       <c r="M15" s="256"/>
       <c r="N15" s="256"/>
       <c r="P15" s="90"/>
@@ -42423,12 +42411,12 @@
       <c r="V19" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="377">
+      <c r="W19" s="373">
         <f>Data!O2</f>
         <v>42370</v>
       </c>
-      <c r="X19" s="377"/>
-      <c r="Y19" s="377"/>
+      <c r="X19" s="373"/>
+      <c r="Y19" s="373"/>
       <c r="Z19" s="261"/>
       <c r="AA19" s="261"/>
     </row>
@@ -42461,12 +42449,12 @@
       <c r="V20" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="W20" s="377">
+      <c r="W20" s="373">
         <f>Data!Y2</f>
         <v>42371</v>
       </c>
-      <c r="X20" s="377"/>
-      <c r="Y20" s="377"/>
+      <c r="X20" s="373"/>
+      <c r="Y20" s="373"/>
       <c r="Z20" s="261"/>
       <c r="AA20" s="261"/>
     </row>
@@ -42499,12 +42487,12 @@
       <c r="V21" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="W21" s="378">
+      <c r="W21" s="374">
         <f>W20+365</f>
         <v>42736</v>
       </c>
-      <c r="X21" s="378"/>
-      <c r="Y21" s="378"/>
+      <c r="X21" s="374"/>
+      <c r="Y21" s="374"/>
       <c r="Z21" s="264"/>
       <c r="AA21" s="264"/>
     </row>
@@ -42846,12 +42834,12 @@
       <c r="G35" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="H35" s="379">
+      <c r="H35" s="375">
         <f>W20+1</f>
         <v>42372</v>
       </c>
-      <c r="I35" s="379"/>
-      <c r="J35" s="379"/>
+      <c r="I35" s="375"/>
+      <c r="J35" s="375"/>
       <c r="K35" s="267"/>
       <c r="L35" s="243"/>
       <c r="M35" s="243"/>
@@ -42904,17 +42892,17 @@
         <v>3</v>
       </c>
       <c r="R36" s="243"/>
-      <c r="S36" s="372" t="str">
+      <c r="S36" s="368" t="str">
         <f>IF(Q36=1,"( Mr.Sombut Srikampa )",IF(Q36=3,"( Mr. Natthaphol Boonmee )"))</f>
         <v>( Mr. Natthaphol Boonmee )</v>
       </c>
-      <c r="T36" s="372"/>
-      <c r="U36" s="372"/>
-      <c r="V36" s="372"/>
-      <c r="W36" s="372"/>
-      <c r="X36" s="372"/>
-      <c r="Y36" s="372"/>
-      <c r="Z36" s="372"/>
+      <c r="T36" s="368"/>
+      <c r="U36" s="368"/>
+      <c r="V36" s="368"/>
+      <c r="W36" s="368"/>
+      <c r="X36" s="368"/>
+      <c r="Y36" s="368"/>
+      <c r="Z36" s="368"/>
       <c r="AA36" s="138"/>
       <c r="AE36" s="266"/>
       <c r="AF36" s="183"/>
@@ -42942,16 +42930,16 @@
       <c r="P37" s="243"/>
       <c r="Q37" s="243"/>
       <c r="R37" s="243"/>
-      <c r="S37" s="373" t="s">
+      <c r="S37" s="369" t="s">
         <v>43</v>
       </c>
-      <c r="T37" s="373"/>
-      <c r="U37" s="373"/>
-      <c r="V37" s="373"/>
-      <c r="W37" s="373"/>
-      <c r="X37" s="373"/>
-      <c r="Y37" s="373"/>
-      <c r="Z37" s="373"/>
+      <c r="T37" s="369"/>
+      <c r="U37" s="369"/>
+      <c r="V37" s="369"/>
+      <c r="W37" s="369"/>
+      <c r="X37" s="369"/>
+      <c r="Y37" s="369"/>
+      <c r="Z37" s="369"/>
       <c r="AA37" s="138"/>
       <c r="AB37" s="88"/>
       <c r="AC37" s="274"/>
@@ -42986,28 +42974,28 @@
       <c r="AA38" s="138"/>
     </row>
     <row r="39" spans="1:36" s="83" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A39" s="374"/>
-      <c r="B39" s="374"/>
-      <c r="C39" s="374"/>
-      <c r="D39" s="374"/>
-      <c r="E39" s="374"/>
-      <c r="F39" s="374"/>
-      <c r="G39" s="374"/>
-      <c r="H39" s="374"/>
-      <c r="I39" s="374"/>
-      <c r="J39" s="374"/>
-      <c r="K39" s="374"/>
-      <c r="L39" s="374"/>
-      <c r="M39" s="374"/>
-      <c r="N39" s="374"/>
-      <c r="O39" s="374"/>
-      <c r="P39" s="374"/>
-      <c r="Q39" s="374"/>
-      <c r="R39" s="374"/>
-      <c r="S39" s="374"/>
-      <c r="T39" s="374"/>
-      <c r="U39" s="374"/>
-      <c r="V39" s="374"/>
+      <c r="A39" s="370"/>
+      <c r="B39" s="370"/>
+      <c r="C39" s="370"/>
+      <c r="D39" s="370"/>
+      <c r="E39" s="370"/>
+      <c r="F39" s="370"/>
+      <c r="G39" s="370"/>
+      <c r="H39" s="370"/>
+      <c r="I39" s="370"/>
+      <c r="J39" s="370"/>
+      <c r="K39" s="370"/>
+      <c r="L39" s="370"/>
+      <c r="M39" s="370"/>
+      <c r="N39" s="370"/>
+      <c r="O39" s="370"/>
+      <c r="P39" s="370"/>
+      <c r="Q39" s="370"/>
+      <c r="R39" s="370"/>
+      <c r="S39" s="370"/>
+      <c r="T39" s="370"/>
+      <c r="U39" s="370"/>
+      <c r="V39" s="370"/>
       <c r="W39" s="146"/>
     </row>
     <row r="40" spans="1:36" ht="18.75" customHeight="1">
@@ -43294,30 +43282,30 @@
     <row r="1" spans="1:22" ht="21.75" customHeight="1"/>
     <row r="2" spans="1:22" ht="13.5" customHeight="1"/>
     <row r="3" spans="1:22" ht="34.5" customHeight="1">
-      <c r="A3" s="385" t="s">
+      <c r="A3" s="376" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="385"/>
-      <c r="C3" s="385"/>
-      <c r="D3" s="385"/>
-      <c r="E3" s="385"/>
-      <c r="F3" s="385"/>
-      <c r="G3" s="385"/>
-      <c r="H3" s="385"/>
-      <c r="I3" s="385"/>
-      <c r="J3" s="385"/>
-      <c r="K3" s="385"/>
-      <c r="L3" s="385"/>
-      <c r="M3" s="385"/>
-      <c r="N3" s="385"/>
-      <c r="O3" s="385"/>
-      <c r="P3" s="385"/>
-      <c r="Q3" s="385"/>
-      <c r="R3" s="385"/>
-      <c r="S3" s="385"/>
-      <c r="T3" s="385"/>
-      <c r="U3" s="385"/>
-      <c r="V3" s="385"/>
+      <c r="B3" s="376"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
+      <c r="G3" s="376"/>
+      <c r="H3" s="376"/>
+      <c r="I3" s="376"/>
+      <c r="J3" s="376"/>
+      <c r="K3" s="376"/>
+      <c r="L3" s="376"/>
+      <c r="M3" s="376"/>
+      <c r="N3" s="376"/>
+      <c r="O3" s="376"/>
+      <c r="P3" s="376"/>
+      <c r="Q3" s="376"/>
+      <c r="R3" s="376"/>
+      <c r="S3" s="376"/>
+      <c r="T3" s="376"/>
+      <c r="U3" s="376"/>
+      <c r="V3" s="376"/>
     </row>
     <row r="4" spans="1:22" ht="18.75" customHeight="1">
       <c r="A4" s="82"/>
@@ -43366,11 +43354,11 @@
       <c r="O5" s="89"/>
       <c r="P5" s="90"/>
       <c r="Q5" s="90"/>
-      <c r="S5" s="384" t="s">
+      <c r="S5" s="398" t="s">
         <v>91</v>
       </c>
-      <c r="T5" s="384"/>
-      <c r="U5" s="384"/>
+      <c r="T5" s="398"/>
+      <c r="U5" s="398"/>
       <c r="V5" s="83"/>
     </row>
     <row r="6" spans="1:22" ht="18" customHeight="1">
@@ -43425,18 +43413,18 @@
       <c r="D8" s="97"/>
       <c r="E8" s="87"/>
       <c r="F8" s="87"/>
-      <c r="G8" s="402" t="s">
+      <c r="G8" s="396" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="402"/>
-      <c r="I8" s="402"/>
-      <c r="J8" s="402"/>
-      <c r="K8" s="402"/>
-      <c r="L8" s="402"/>
-      <c r="M8" s="402"/>
-      <c r="N8" s="402"/>
-      <c r="O8" s="402"/>
-      <c r="P8" s="402"/>
+      <c r="H8" s="396"/>
+      <c r="I8" s="396"/>
+      <c r="J8" s="396"/>
+      <c r="K8" s="396"/>
+      <c r="L8" s="396"/>
+      <c r="M8" s="396"/>
+      <c r="N8" s="396"/>
+      <c r="O8" s="396"/>
+      <c r="P8" s="396"/>
       <c r="Q8" s="100"/>
       <c r="R8" s="100"/>
       <c r="S8" s="100"/>
@@ -43451,16 +43439,16 @@
       <c r="D9" s="97"/>
       <c r="E9" s="87"/>
       <c r="F9" s="87"/>
-      <c r="G9" s="402"/>
-      <c r="H9" s="402"/>
-      <c r="I9" s="402"/>
-      <c r="J9" s="402"/>
-      <c r="K9" s="402"/>
-      <c r="L9" s="402"/>
-      <c r="M9" s="402"/>
-      <c r="N9" s="402"/>
-      <c r="O9" s="402"/>
-      <c r="P9" s="402"/>
+      <c r="G9" s="396"/>
+      <c r="H9" s="396"/>
+      <c r="I9" s="396"/>
+      <c r="J9" s="396"/>
+      <c r="K9" s="396"/>
+      <c r="L9" s="396"/>
+      <c r="M9" s="396"/>
+      <c r="N9" s="396"/>
+      <c r="O9" s="396"/>
+      <c r="P9" s="396"/>
       <c r="Q9" s="100"/>
       <c r="R9" s="100"/>
       <c r="S9" s="100"/>
@@ -43494,70 +43482,70 @@
     </row>
     <row r="11" spans="1:22" ht="23.1" customHeight="1">
       <c r="A11" s="84"/>
-      <c r="B11" s="380" t="s">
+      <c r="B11" s="395" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="381"/>
-      <c r="D11" s="381"/>
-      <c r="E11" s="381"/>
-      <c r="F11" s="381"/>
-      <c r="G11" s="382"/>
-      <c r="H11" s="380" t="s">
+      <c r="C11" s="393"/>
+      <c r="D11" s="393"/>
+      <c r="E11" s="393"/>
+      <c r="F11" s="393"/>
+      <c r="G11" s="394"/>
+      <c r="H11" s="395" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="381"/>
-      <c r="J11" s="382"/>
-      <c r="K11" s="380" t="s">
+      <c r="I11" s="393"/>
+      <c r="J11" s="394"/>
+      <c r="K11" s="395" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="381"/>
-      <c r="M11" s="382"/>
-      <c r="N11" s="380" t="s">
+      <c r="L11" s="393"/>
+      <c r="M11" s="394"/>
+      <c r="N11" s="395" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="381"/>
-      <c r="P11" s="381"/>
-      <c r="Q11" s="382"/>
-      <c r="R11" s="381" t="s">
+      <c r="O11" s="393"/>
+      <c r="P11" s="393"/>
+      <c r="Q11" s="394"/>
+      <c r="R11" s="393" t="s">
         <v>47</v>
       </c>
-      <c r="S11" s="381"/>
-      <c r="T11" s="381"/>
-      <c r="U11" s="382"/>
+      <c r="S11" s="393"/>
+      <c r="T11" s="393"/>
+      <c r="U11" s="394"/>
       <c r="V11" s="83"/>
     </row>
     <row r="12" spans="1:22" ht="23.1" customHeight="1">
       <c r="A12" s="84"/>
-      <c r="B12" s="391" t="s">
+      <c r="B12" s="382" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="392"/>
-      <c r="D12" s="392"/>
-      <c r="E12" s="392"/>
-      <c r="F12" s="392"/>
-      <c r="G12" s="392"/>
-      <c r="H12" s="393" t="s">
+      <c r="C12" s="383"/>
+      <c r="D12" s="383"/>
+      <c r="E12" s="383"/>
+      <c r="F12" s="383"/>
+      <c r="G12" s="383"/>
+      <c r="H12" s="384" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="394"/>
-      <c r="J12" s="395"/>
-      <c r="K12" s="393">
+      <c r="I12" s="385"/>
+      <c r="J12" s="386"/>
+      <c r="K12" s="384">
         <v>60711</v>
       </c>
-      <c r="L12" s="394"/>
-      <c r="M12" s="395"/>
-      <c r="N12" s="396" t="s">
+      <c r="L12" s="385"/>
+      <c r="M12" s="386"/>
+      <c r="N12" s="387" t="s">
         <v>95</v>
       </c>
-      <c r="O12" s="397"/>
-      <c r="P12" s="397"/>
-      <c r="Q12" s="398"/>
-      <c r="R12" s="399">
+      <c r="O12" s="388"/>
+      <c r="P12" s="388"/>
+      <c r="Q12" s="389"/>
+      <c r="R12" s="390">
         <v>42336</v>
       </c>
-      <c r="S12" s="400"/>
-      <c r="T12" s="400"/>
-      <c r="U12" s="401"/>
+      <c r="S12" s="391"/>
+      <c r="T12" s="391"/>
+      <c r="U12" s="392"/>
       <c r="V12" s="118"/>
     </row>
     <row r="13" spans="1:22" ht="18" customHeight="1">
@@ -43696,10 +43684,10 @@
       <c r="G18" s="87"/>
       <c r="H18" s="87"/>
       <c r="I18" s="115"/>
-      <c r="J18" s="390"/>
-      <c r="K18" s="389"/>
-      <c r="L18" s="389"/>
-      <c r="M18" s="389"/>
+      <c r="J18" s="381"/>
+      <c r="K18" s="380"/>
+      <c r="L18" s="380"/>
+      <c r="M18" s="380"/>
       <c r="N18" s="83"/>
       <c r="O18" s="116"/>
       <c r="P18" s="116"/>
@@ -43720,10 +43708,10 @@
       <c r="G19" s="87"/>
       <c r="H19" s="87"/>
       <c r="I19" s="115"/>
-      <c r="J19" s="389"/>
-      <c r="K19" s="389"/>
-      <c r="L19" s="389"/>
-      <c r="M19" s="389"/>
+      <c r="J19" s="380"/>
+      <c r="K19" s="380"/>
+      <c r="L19" s="380"/>
+      <c r="M19" s="380"/>
       <c r="N19" s="83"/>
       <c r="O19" s="116"/>
       <c r="P19" s="116"/>
@@ -44172,16 +44160,16 @@
       <c r="C38" s="111"/>
       <c r="D38" s="111"/>
       <c r="E38" s="111"/>
-      <c r="F38" s="386"/>
-      <c r="G38" s="386"/>
-      <c r="H38" s="386"/>
-      <c r="I38" s="386"/>
+      <c r="F38" s="377"/>
+      <c r="G38" s="377"/>
+      <c r="H38" s="377"/>
+      <c r="I38" s="377"/>
       <c r="J38" s="143"/>
       <c r="K38" s="111"/>
-      <c r="L38" s="387"/>
-      <c r="M38" s="387"/>
-      <c r="N38" s="387"/>
-      <c r="O38" s="387"/>
+      <c r="L38" s="378"/>
+      <c r="M38" s="378"/>
+      <c r="N38" s="378"/>
+      <c r="O38" s="378"/>
       <c r="P38" s="89"/>
       <c r="Q38" s="89"/>
       <c r="R38" s="89"/>
@@ -44230,11 +44218,11 @@
       <c r="M40" s="103"/>
       <c r="N40" s="103"/>
       <c r="O40" s="103"/>
-      <c r="P40" s="388"/>
-      <c r="Q40" s="388"/>
-      <c r="R40" s="388"/>
-      <c r="S40" s="388"/>
-      <c r="T40" s="388"/>
+      <c r="P40" s="379"/>
+      <c r="Q40" s="379"/>
+      <c r="R40" s="379"/>
+      <c r="S40" s="379"/>
+      <c r="T40" s="379"/>
       <c r="U40" s="138"/>
       <c r="V40" s="138"/>
     </row>
@@ -44242,11 +44230,11 @@
       <c r="A41" s="84"/>
       <c r="B41" s="83"/>
       <c r="C41" s="83"/>
-      <c r="D41" s="383"/>
-      <c r="E41" s="383"/>
-      <c r="F41" s="383"/>
-      <c r="G41" s="383"/>
-      <c r="H41" s="383"/>
+      <c r="D41" s="397"/>
+      <c r="E41" s="397"/>
+      <c r="F41" s="397"/>
+      <c r="G41" s="397"/>
+      <c r="H41" s="397"/>
       <c r="I41" s="83"/>
       <c r="J41" s="83"/>
       <c r="K41" s="103"/>
@@ -44263,31 +44251,35 @@
       <c r="V41" s="138"/>
     </row>
     <row r="42" spans="1:22" ht="15">
-      <c r="A42" s="374"/>
-      <c r="B42" s="374"/>
-      <c r="C42" s="374"/>
-      <c r="D42" s="374"/>
-      <c r="E42" s="374"/>
-      <c r="F42" s="374"/>
-      <c r="G42" s="374"/>
-      <c r="H42" s="374"/>
-      <c r="I42" s="374"/>
-      <c r="J42" s="374"/>
-      <c r="K42" s="374"/>
-      <c r="L42" s="374"/>
-      <c r="M42" s="374"/>
-      <c r="N42" s="374"/>
-      <c r="O42" s="374"/>
-      <c r="P42" s="374"/>
-      <c r="Q42" s="374"/>
-      <c r="R42" s="374"/>
-      <c r="S42" s="374"/>
-      <c r="T42" s="374"/>
+      <c r="A42" s="370"/>
+      <c r="B42" s="370"/>
+      <c r="C42" s="370"/>
+      <c r="D42" s="370"/>
+      <c r="E42" s="370"/>
+      <c r="F42" s="370"/>
+      <c r="G42" s="370"/>
+      <c r="H42" s="370"/>
+      <c r="I42" s="370"/>
+      <c r="J42" s="370"/>
+      <c r="K42" s="370"/>
+      <c r="L42" s="370"/>
+      <c r="M42" s="370"/>
+      <c r="N42" s="370"/>
+      <c r="O42" s="370"/>
+      <c r="P42" s="370"/>
+      <c r="Q42" s="370"/>
+      <c r="R42" s="370"/>
+      <c r="S42" s="370"/>
+      <c r="T42" s="370"/>
       <c r="U42" s="146"/>
       <c r="V42" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="A42:T42"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="A3:V3"/>
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="L38:O38"/>
@@ -44304,10 +44296,6 @@
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="G8:P9"/>
     <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="A42:T42"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.98425196850393704" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -44381,30 +44369,30 @@
       <c r="U2" s="147"/>
     </row>
     <row r="3" spans="1:35" ht="34.5" customHeight="1">
-      <c r="A3" s="430" t="s">
+      <c r="A3" s="408" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="430"/>
-      <c r="C3" s="430"/>
-      <c r="D3" s="430"/>
-      <c r="E3" s="430"/>
-      <c r="F3" s="430"/>
-      <c r="G3" s="430"/>
-      <c r="H3" s="430"/>
-      <c r="I3" s="430"/>
-      <c r="J3" s="430"/>
-      <c r="K3" s="430"/>
-      <c r="L3" s="430"/>
-      <c r="M3" s="430"/>
-      <c r="N3" s="430"/>
-      <c r="O3" s="430"/>
-      <c r="P3" s="430"/>
-      <c r="Q3" s="430"/>
-      <c r="R3" s="430"/>
-      <c r="S3" s="430"/>
-      <c r="T3" s="430"/>
-      <c r="U3" s="430"/>
-      <c r="V3" s="430"/>
+      <c r="B3" s="408"/>
+      <c r="C3" s="408"/>
+      <c r="D3" s="408"/>
+      <c r="E3" s="408"/>
+      <c r="F3" s="408"/>
+      <c r="G3" s="408"/>
+      <c r="H3" s="408"/>
+      <c r="I3" s="408"/>
+      <c r="J3" s="408"/>
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="408"/>
+      <c r="N3" s="408"/>
+      <c r="O3" s="408"/>
+      <c r="P3" s="408"/>
+      <c r="Q3" s="408"/>
+      <c r="R3" s="408"/>
+      <c r="S3" s="408"/>
+      <c r="T3" s="408"/>
+      <c r="U3" s="408"/>
+      <c r="V3" s="408"/>
     </row>
     <row r="4" spans="1:35" ht="18.75" customHeight="1">
       <c r="A4" s="147"/>
@@ -44437,13 +44425,13 @@
       <c r="C5" s="152"/>
       <c r="D5" s="152"/>
       <c r="E5" s="149"/>
-      <c r="F5" s="437" t="str">
+      <c r="F5" s="415" t="str">
         <f>Report!G5</f>
         <v>SPR16010011-1</v>
       </c>
-      <c r="G5" s="437"/>
-      <c r="H5" s="437"/>
-      <c r="I5" s="437"/>
+      <c r="G5" s="415"/>
+      <c r="H5" s="415"/>
+      <c r="I5" s="415"/>
       <c r="J5" s="147"/>
       <c r="K5" s="147"/>
       <c r="L5" s="147"/>
@@ -44500,10 +44488,10 @@
       <c r="M7" s="147"/>
       <c r="N7" s="147"/>
       <c r="O7" s="148"/>
-      <c r="P7" s="438" t="s">
+      <c r="P7" s="416" t="s">
         <v>123</v>
       </c>
-      <c r="Q7" s="438"/>
+      <c r="Q7" s="416"/>
       <c r="R7" s="289" t="s">
         <v>10</v>
       </c>
@@ -44515,29 +44503,29 @@
       <c r="A8" s="228"/>
       <c r="B8" s="228"/>
       <c r="C8" s="228"/>
-      <c r="D8" s="431" t="s">
+      <c r="D8" s="409" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="432"/>
-      <c r="F8" s="432"/>
-      <c r="G8" s="433"/>
-      <c r="H8" s="432" t="s">
+      <c r="E8" s="410"/>
+      <c r="F8" s="410"/>
+      <c r="G8" s="411"/>
+      <c r="H8" s="410" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="432"/>
-      <c r="J8" s="432"/>
-      <c r="K8" s="433"/>
-      <c r="L8" s="439" t="s">
+      <c r="I8" s="410"/>
+      <c r="J8" s="410"/>
+      <c r="K8" s="411"/>
+      <c r="L8" s="417" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="440"/>
-      <c r="N8" s="441"/>
-      <c r="O8" s="445" t="s">
+      <c r="M8" s="418"/>
+      <c r="N8" s="419"/>
+      <c r="O8" s="423" t="s">
         <v>124</v>
       </c>
-      <c r="P8" s="446"/>
-      <c r="Q8" s="446"/>
-      <c r="R8" s="447"/>
+      <c r="P8" s="424"/>
+      <c r="Q8" s="424"/>
+      <c r="R8" s="425"/>
       <c r="S8" s="228"/>
       <c r="T8" s="228"/>
       <c r="U8" s="228"/>
@@ -44546,21 +44534,21 @@
       <c r="A9" s="228"/>
       <c r="B9" s="229"/>
       <c r="C9" s="229"/>
-      <c r="D9" s="434"/>
-      <c r="E9" s="435"/>
-      <c r="F9" s="435"/>
-      <c r="G9" s="436"/>
-      <c r="H9" s="435"/>
-      <c r="I9" s="435"/>
-      <c r="J9" s="435"/>
-      <c r="K9" s="436"/>
-      <c r="L9" s="442"/>
-      <c r="M9" s="443"/>
-      <c r="N9" s="444"/>
-      <c r="O9" s="448"/>
-      <c r="P9" s="449"/>
-      <c r="Q9" s="449"/>
-      <c r="R9" s="450"/>
+      <c r="D9" s="412"/>
+      <c r="E9" s="413"/>
+      <c r="F9" s="413"/>
+      <c r="G9" s="414"/>
+      <c r="H9" s="413"/>
+      <c r="I9" s="413"/>
+      <c r="J9" s="413"/>
+      <c r="K9" s="414"/>
+      <c r="L9" s="420"/>
+      <c r="M9" s="421"/>
+      <c r="N9" s="422"/>
+      <c r="O9" s="426"/>
+      <c r="P9" s="427"/>
+      <c r="Q9" s="427"/>
+      <c r="R9" s="428"/>
       <c r="S9" s="228"/>
       <c r="T9" s="228"/>
       <c r="U9" s="228"/>
@@ -44569,33 +44557,33 @@
       <c r="A10" s="228"/>
       <c r="B10" s="230"/>
       <c r="C10" s="230"/>
-      <c r="D10" s="424">
+      <c r="D10" s="429">
         <f>Data!B16</f>
         <v>0</v>
       </c>
-      <c r="E10" s="425"/>
-      <c r="F10" s="425"/>
-      <c r="G10" s="426"/>
-      <c r="H10" s="419">
+      <c r="E10" s="430"/>
+      <c r="F10" s="430"/>
+      <c r="G10" s="431"/>
+      <c r="H10" s="403">
         <f>Data!Q16</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="I10" s="419"/>
-      <c r="J10" s="419"/>
-      <c r="K10" s="420"/>
-      <c r="L10" s="451">
+      <c r="I10" s="403"/>
+      <c r="J10" s="403"/>
+      <c r="K10" s="404"/>
+      <c r="L10" s="402">
         <f>Data!X16</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="M10" s="419"/>
-      <c r="N10" s="420"/>
-      <c r="O10" s="416">
+      <c r="M10" s="403"/>
+      <c r="N10" s="404"/>
+      <c r="O10" s="432">
         <f>'Uncertainty Budget 0 to 25mm'!O8</f>
         <v>0.82827878797800292</v>
       </c>
-      <c r="P10" s="417"/>
-      <c r="Q10" s="417"/>
-      <c r="R10" s="418"/>
+      <c r="P10" s="433"/>
+      <c r="Q10" s="433"/>
+      <c r="R10" s="434"/>
       <c r="S10" s="228"/>
       <c r="T10" s="228"/>
       <c r="U10" s="228"/>
@@ -44604,33 +44592,33 @@
       <c r="A11" s="228"/>
       <c r="B11" s="230"/>
       <c r="C11" s="230"/>
-      <c r="D11" s="427">
+      <c r="D11" s="405">
         <f>Data!B17</f>
         <v>2.5</v>
       </c>
-      <c r="E11" s="428"/>
-      <c r="F11" s="428"/>
-      <c r="G11" s="429"/>
-      <c r="H11" s="421">
+      <c r="E11" s="406"/>
+      <c r="F11" s="406"/>
+      <c r="G11" s="407"/>
+      <c r="H11" s="399">
         <f>Data!Q17</f>
         <v>2.5004999999999997</v>
       </c>
-      <c r="I11" s="422"/>
-      <c r="J11" s="422"/>
-      <c r="K11" s="423"/>
-      <c r="L11" s="421">
+      <c r="I11" s="400"/>
+      <c r="J11" s="400"/>
+      <c r="K11" s="401"/>
+      <c r="L11" s="399">
         <f>Data!X17</f>
         <v>4.9999999999972289E-4</v>
       </c>
-      <c r="M11" s="422"/>
-      <c r="N11" s="423"/>
-      <c r="O11" s="413">
+      <c r="M11" s="400"/>
+      <c r="N11" s="401"/>
+      <c r="O11" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O9</f>
         <v>1.5318952855025763</v>
       </c>
-      <c r="P11" s="414"/>
-      <c r="Q11" s="414"/>
-      <c r="R11" s="415"/>
+      <c r="P11" s="436"/>
+      <c r="Q11" s="436"/>
+      <c r="R11" s="437"/>
       <c r="S11" s="228"/>
       <c r="T11" s="228"/>
       <c r="U11" s="228"/>
@@ -44639,33 +44627,33 @@
       <c r="A12" s="228"/>
       <c r="B12" s="230"/>
       <c r="C12" s="230"/>
-      <c r="D12" s="427">
+      <c r="D12" s="405">
         <f>Data!B18</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="E12" s="428"/>
-      <c r="F12" s="428"/>
-      <c r="G12" s="429"/>
-      <c r="H12" s="421">
+      <c r="E12" s="406"/>
+      <c r="F12" s="406"/>
+      <c r="G12" s="407"/>
+      <c r="H12" s="399">
         <f>Data!Q18</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="I12" s="422"/>
-      <c r="J12" s="422"/>
-      <c r="K12" s="423"/>
-      <c r="L12" s="421">
+      <c r="I12" s="400"/>
+      <c r="J12" s="400"/>
+      <c r="K12" s="401"/>
+      <c r="L12" s="399">
         <f>Data!X18</f>
         <v>0</v>
       </c>
-      <c r="M12" s="422"/>
-      <c r="N12" s="423"/>
-      <c r="O12" s="413">
+      <c r="M12" s="400"/>
+      <c r="N12" s="401"/>
+      <c r="O12" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O10</f>
         <v>0.58439692276169053</v>
       </c>
-      <c r="P12" s="414"/>
-      <c r="Q12" s="414"/>
-      <c r="R12" s="415"/>
+      <c r="P12" s="436"/>
+      <c r="Q12" s="436"/>
+      <c r="R12" s="437"/>
       <c r="S12" s="228"/>
       <c r="T12" s="228"/>
       <c r="U12" s="228"/>
@@ -44674,33 +44662,33 @@
       <c r="A13" s="228"/>
       <c r="B13" s="230"/>
       <c r="C13" s="230"/>
-      <c r="D13" s="427">
+      <c r="D13" s="405">
         <f>Data!B19</f>
         <v>7.7</v>
       </c>
-      <c r="E13" s="428"/>
-      <c r="F13" s="428"/>
-      <c r="G13" s="429"/>
-      <c r="H13" s="421">
+      <c r="E13" s="406"/>
+      <c r="F13" s="406"/>
+      <c r="G13" s="407"/>
+      <c r="H13" s="399">
         <f>Data!Q19</f>
         <v>7.7</v>
       </c>
-      <c r="I13" s="422"/>
-      <c r="J13" s="422"/>
-      <c r="K13" s="423"/>
-      <c r="L13" s="421">
+      <c r="I13" s="400"/>
+      <c r="J13" s="400"/>
+      <c r="K13" s="401"/>
+      <c r="L13" s="399">
         <f>Data!X19</f>
         <v>0</v>
       </c>
-      <c r="M13" s="422"/>
-      <c r="N13" s="423"/>
-      <c r="O13" s="413">
+      <c r="M13" s="400"/>
+      <c r="N13" s="401"/>
+      <c r="O13" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O11</f>
         <v>0.58939641724960179</v>
       </c>
-      <c r="P13" s="414"/>
-      <c r="Q13" s="414"/>
-      <c r="R13" s="415"/>
+      <c r="P13" s="436"/>
+      <c r="Q13" s="436"/>
+      <c r="R13" s="437"/>
       <c r="S13" s="228"/>
       <c r="T13" s="228"/>
       <c r="U13" s="228"/>
@@ -44709,33 +44697,33 @@
       <c r="A14" s="228"/>
       <c r="B14" s="230"/>
       <c r="C14" s="230"/>
-      <c r="D14" s="427">
+      <c r="D14" s="405">
         <f>Data!B20</f>
         <v>10.3</v>
       </c>
-      <c r="E14" s="428"/>
-      <c r="F14" s="428"/>
-      <c r="G14" s="429"/>
-      <c r="H14" s="421">
+      <c r="E14" s="406"/>
+      <c r="F14" s="406"/>
+      <c r="G14" s="407"/>
+      <c r="H14" s="399">
         <f>Data!Q20</f>
         <v>10.3</v>
       </c>
-      <c r="I14" s="422"/>
-      <c r="J14" s="422"/>
-      <c r="K14" s="423"/>
-      <c r="L14" s="421">
+      <c r="I14" s="400"/>
+      <c r="J14" s="400"/>
+      <c r="K14" s="401"/>
+      <c r="L14" s="399">
         <f>Data!X20</f>
         <v>0</v>
       </c>
-      <c r="M14" s="422"/>
-      <c r="N14" s="423"/>
-      <c r="O14" s="413">
+      <c r="M14" s="400"/>
+      <c r="N14" s="401"/>
+      <c r="O14" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O12</f>
         <v>0.59744500723218597</v>
       </c>
-      <c r="P14" s="414"/>
-      <c r="Q14" s="414"/>
-      <c r="R14" s="415"/>
+      <c r="P14" s="436"/>
+      <c r="Q14" s="436"/>
+      <c r="R14" s="437"/>
       <c r="S14" s="228"/>
       <c r="T14" s="228"/>
       <c r="U14" s="228"/>
@@ -44745,33 +44733,33 @@
       <c r="A15" s="228"/>
       <c r="B15" s="230"/>
       <c r="C15" s="230"/>
-      <c r="D15" s="427">
+      <c r="D15" s="405">
         <f>Data!B21</f>
         <v>12.9</v>
       </c>
-      <c r="E15" s="428"/>
-      <c r="F15" s="428"/>
-      <c r="G15" s="429"/>
-      <c r="H15" s="421">
+      <c r="E15" s="406"/>
+      <c r="F15" s="406"/>
+      <c r="G15" s="407"/>
+      <c r="H15" s="399">
         <f>Data!Q21</f>
         <v>12.9</v>
       </c>
-      <c r="I15" s="422"/>
-      <c r="J15" s="422"/>
-      <c r="K15" s="423"/>
-      <c r="L15" s="421">
+      <c r="I15" s="400"/>
+      <c r="J15" s="400"/>
+      <c r="K15" s="401"/>
+      <c r="L15" s="399">
         <f>Data!X21</f>
         <v>0</v>
       </c>
-      <c r="M15" s="422"/>
-      <c r="N15" s="423"/>
-      <c r="O15" s="413">
+      <c r="M15" s="400"/>
+      <c r="N15" s="401"/>
+      <c r="O15" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O13</f>
         <v>0.6062812576134391</v>
       </c>
-      <c r="P15" s="414"/>
-      <c r="Q15" s="414"/>
-      <c r="R15" s="415"/>
+      <c r="P15" s="436"/>
+      <c r="Q15" s="436"/>
+      <c r="R15" s="437"/>
       <c r="S15" s="228"/>
       <c r="T15" s="228"/>
       <c r="U15" s="228"/>
@@ -44780,33 +44768,33 @@
       <c r="A16" s="228"/>
       <c r="B16" s="230"/>
       <c r="C16" s="230"/>
-      <c r="D16" s="427">
+      <c r="D16" s="405">
         <f>Data!B22</f>
         <v>15</v>
       </c>
-      <c r="E16" s="428"/>
-      <c r="F16" s="428"/>
-      <c r="G16" s="429"/>
-      <c r="H16" s="421">
+      <c r="E16" s="406"/>
+      <c r="F16" s="406"/>
+      <c r="G16" s="407"/>
+      <c r="H16" s="399">
         <f>Data!Q22</f>
         <v>15</v>
       </c>
-      <c r="I16" s="422"/>
-      <c r="J16" s="422"/>
-      <c r="K16" s="423"/>
-      <c r="L16" s="421">
+      <c r="I16" s="400"/>
+      <c r="J16" s="400"/>
+      <c r="K16" s="401"/>
+      <c r="L16" s="399">
         <f>Data!X22</f>
         <v>0</v>
       </c>
-      <c r="M16" s="422"/>
-      <c r="N16" s="423"/>
-      <c r="O16" s="413">
+      <c r="M16" s="400"/>
+      <c r="N16" s="401"/>
+      <c r="O16" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O14</f>
         <v>0.6147424935152388</v>
       </c>
-      <c r="P16" s="414"/>
-      <c r="Q16" s="414"/>
-      <c r="R16" s="415"/>
+      <c r="P16" s="436"/>
+      <c r="Q16" s="436"/>
+      <c r="R16" s="437"/>
       <c r="S16" s="228"/>
       <c r="T16" s="228"/>
       <c r="U16" s="228"/>
@@ -44815,33 +44803,33 @@
       <c r="A17" s="228"/>
       <c r="B17" s="230"/>
       <c r="C17" s="230"/>
-      <c r="D17" s="427">
+      <c r="D17" s="405">
         <f>Data!B23</f>
         <v>17.600000000000001</v>
       </c>
-      <c r="E17" s="428"/>
-      <c r="F17" s="428"/>
-      <c r="G17" s="429"/>
-      <c r="H17" s="421">
+      <c r="E17" s="406"/>
+      <c r="F17" s="406"/>
+      <c r="G17" s="407"/>
+      <c r="H17" s="399">
         <f>Data!Q23</f>
         <v>17.600000000000001</v>
       </c>
-      <c r="I17" s="422"/>
-      <c r="J17" s="422"/>
-      <c r="K17" s="423"/>
-      <c r="L17" s="421">
+      <c r="I17" s="400"/>
+      <c r="J17" s="400"/>
+      <c r="K17" s="401"/>
+      <c r="L17" s="399">
         <f>Data!X23</f>
         <v>0</v>
       </c>
-      <c r="M17" s="422"/>
-      <c r="N17" s="423"/>
-      <c r="O17" s="413">
+      <c r="M17" s="400"/>
+      <c r="N17" s="401"/>
+      <c r="O17" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O15</f>
         <v>0.62678093993568984</v>
       </c>
-      <c r="P17" s="414"/>
-      <c r="Q17" s="414"/>
-      <c r="R17" s="415"/>
+      <c r="P17" s="436"/>
+      <c r="Q17" s="436"/>
+      <c r="R17" s="437"/>
       <c r="S17" s="228"/>
       <c r="T17" s="228"/>
       <c r="U17" s="228"/>
@@ -44850,33 +44838,33 @@
       <c r="A18" s="228"/>
       <c r="B18" s="230"/>
       <c r="C18" s="230"/>
-      <c r="D18" s="427">
+      <c r="D18" s="405">
         <f>Data!B24</f>
         <v>20.2</v>
       </c>
-      <c r="E18" s="428"/>
-      <c r="F18" s="428"/>
-      <c r="G18" s="429"/>
-      <c r="H18" s="421">
+      <c r="E18" s="406"/>
+      <c r="F18" s="406"/>
+      <c r="G18" s="407"/>
+      <c r="H18" s="399">
         <f>Data!Q24</f>
         <v>20.2</v>
       </c>
-      <c r="I18" s="422"/>
-      <c r="J18" s="422"/>
-      <c r="K18" s="423"/>
-      <c r="L18" s="421">
+      <c r="I18" s="400"/>
+      <c r="J18" s="400"/>
+      <c r="K18" s="401"/>
+      <c r="L18" s="399">
         <f>Data!X24</f>
         <v>0</v>
       </c>
-      <c r="M18" s="422"/>
-      <c r="N18" s="423"/>
-      <c r="O18" s="413">
+      <c r="M18" s="400"/>
+      <c r="N18" s="401"/>
+      <c r="O18" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O16</f>
         <v>0.64045638935579885</v>
       </c>
-      <c r="P18" s="414"/>
-      <c r="Q18" s="414"/>
-      <c r="R18" s="415"/>
+      <c r="P18" s="436"/>
+      <c r="Q18" s="436"/>
+      <c r="R18" s="437"/>
       <c r="S18" s="189"/>
       <c r="T18" s="231"/>
       <c r="U18" s="228"/>
@@ -44885,33 +44873,33 @@
       <c r="A19" s="228"/>
       <c r="B19" s="230"/>
       <c r="C19" s="230"/>
-      <c r="D19" s="427">
+      <c r="D19" s="405">
         <f>Data!B25</f>
         <v>22.8</v>
       </c>
-      <c r="E19" s="428"/>
-      <c r="F19" s="428"/>
-      <c r="G19" s="429"/>
-      <c r="H19" s="421">
+      <c r="E19" s="406"/>
+      <c r="F19" s="406"/>
+      <c r="G19" s="407"/>
+      <c r="H19" s="399">
         <f>Data!Q25</f>
         <v>22.8</v>
       </c>
-      <c r="I19" s="422"/>
-      <c r="J19" s="422"/>
-      <c r="K19" s="423"/>
-      <c r="L19" s="421">
+      <c r="I19" s="400"/>
+      <c r="J19" s="400"/>
+      <c r="K19" s="401"/>
+      <c r="L19" s="399">
         <f>Data!X25</f>
         <v>0</v>
       </c>
-      <c r="M19" s="422"/>
-      <c r="N19" s="423"/>
-      <c r="O19" s="413">
+      <c r="M19" s="400"/>
+      <c r="N19" s="401"/>
+      <c r="O19" s="435">
         <f>'Uncertainty Budget 0 to 25mm'!O17</f>
         <v>0.65566641925092772</v>
       </c>
-      <c r="P19" s="414"/>
-      <c r="Q19" s="414"/>
-      <c r="R19" s="415"/>
+      <c r="P19" s="436"/>
+      <c r="Q19" s="436"/>
+      <c r="R19" s="437"/>
       <c r="S19" s="189"/>
       <c r="T19" s="231"/>
       <c r="U19" s="228"/>
@@ -44920,33 +44908,33 @@
       <c r="A20" s="228"/>
       <c r="B20" s="228"/>
       <c r="C20" s="228"/>
-      <c r="D20" s="406">
+      <c r="D20" s="441">
         <f>Data!B26</f>
         <v>25</v>
       </c>
-      <c r="E20" s="407"/>
-      <c r="F20" s="407"/>
-      <c r="G20" s="408"/>
-      <c r="H20" s="409">
+      <c r="E20" s="442"/>
+      <c r="F20" s="442"/>
+      <c r="G20" s="443"/>
+      <c r="H20" s="444">
         <f>Data!Q26</f>
         <v>25</v>
       </c>
-      <c r="I20" s="409"/>
-      <c r="J20" s="409"/>
-      <c r="K20" s="410"/>
-      <c r="L20" s="411">
+      <c r="I20" s="444"/>
+      <c r="J20" s="444"/>
+      <c r="K20" s="445"/>
+      <c r="L20" s="446">
         <f>Data!X26</f>
         <v>0</v>
       </c>
-      <c r="M20" s="409"/>
-      <c r="N20" s="410"/>
-      <c r="O20" s="403">
+      <c r="M20" s="444"/>
+      <c r="N20" s="445"/>
+      <c r="O20" s="438">
         <f>'Uncertainty Budget 0 to 25mm'!O18</f>
         <v>0.6696578728475211</v>
       </c>
-      <c r="P20" s="404"/>
-      <c r="Q20" s="404"/>
-      <c r="R20" s="405"/>
+      <c r="P20" s="439"/>
+      <c r="Q20" s="439"/>
+      <c r="R20" s="440"/>
       <c r="S20" s="231"/>
       <c r="T20" s="232"/>
       <c r="U20" s="189"/>
@@ -45043,30 +45031,30 @@
       <c r="X24" s="285"/>
     </row>
     <row r="25" spans="1:24" s="286" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A25" s="412" t="s">
+      <c r="A25" s="447" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="412"/>
-      <c r="C25" s="412"/>
-      <c r="D25" s="412"/>
-      <c r="E25" s="412"/>
-      <c r="F25" s="412"/>
-      <c r="G25" s="412"/>
-      <c r="H25" s="412"/>
-      <c r="I25" s="412"/>
-      <c r="J25" s="412"/>
-      <c r="K25" s="412"/>
-      <c r="L25" s="412"/>
-      <c r="M25" s="412"/>
-      <c r="N25" s="412"/>
-      <c r="O25" s="412"/>
-      <c r="P25" s="412"/>
-      <c r="Q25" s="412"/>
-      <c r="R25" s="412"/>
-      <c r="S25" s="412"/>
-      <c r="T25" s="412"/>
-      <c r="U25" s="412"/>
-      <c r="V25" s="412"/>
+      <c r="B25" s="447"/>
+      <c r="C25" s="447"/>
+      <c r="D25" s="447"/>
+      <c r="E25" s="447"/>
+      <c r="F25" s="447"/>
+      <c r="G25" s="447"/>
+      <c r="H25" s="447"/>
+      <c r="I25" s="447"/>
+      <c r="J25" s="447"/>
+      <c r="K25" s="447"/>
+      <c r="L25" s="447"/>
+      <c r="M25" s="447"/>
+      <c r="N25" s="447"/>
+      <c r="O25" s="447"/>
+      <c r="P25" s="447"/>
+      <c r="Q25" s="447"/>
+      <c r="R25" s="447"/>
+      <c r="S25" s="447"/>
+      <c r="T25" s="447"/>
+      <c r="U25" s="447"/>
+      <c r="V25" s="447"/>
       <c r="W25" s="294"/>
       <c r="X25" s="294"/>
     </row>
@@ -45971,21 +45959,36 @@
     <row r="198" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="A25:V25"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
     <mergeCell ref="A3:V3"/>
     <mergeCell ref="D8:G9"/>
     <mergeCell ref="H8:K9"/>
@@ -45993,36 +45996,21 @@
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="L8:N9"/>
     <mergeCell ref="O8:R9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="A25:V25"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L10:N10"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.98425196850393704" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -46039,7 +46027,7 @@
   </sheetPr>
   <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
@@ -46498,22 +46486,22 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="33" customHeight="1">
-      <c r="B2" s="456" t="s">
+      <c r="B2" s="448" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="456"/>
-      <c r="D2" s="456"/>
-      <c r="E2" s="456"/>
-      <c r="F2" s="456"/>
-      <c r="G2" s="456"/>
-      <c r="H2" s="456"/>
-      <c r="I2" s="456"/>
-      <c r="J2" s="456"/>
-      <c r="K2" s="456"/>
-      <c r="L2" s="456"/>
-      <c r="M2" s="456"/>
-      <c r="N2" s="456"/>
-      <c r="O2" s="456"/>
+      <c r="C2" s="448"/>
+      <c r="D2" s="448"/>
+      <c r="E2" s="448"/>
+      <c r="F2" s="448"/>
+      <c r="G2" s="448"/>
+      <c r="H2" s="448"/>
+      <c r="I2" s="448"/>
+      <c r="J2" s="448"/>
+      <c r="K2" s="448"/>
+      <c r="L2" s="448"/>
+      <c r="M2" s="448"/>
+      <c r="N2" s="448"/>
+      <c r="O2" s="448"/>
     </row>
     <row r="3" spans="1:16" ht="9.75" customHeight="1">
       <c r="B3" s="5"/>
@@ -46530,11 +46518,11 @@
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="18" customHeight="1">
-      <c r="B4" s="457"/>
-      <c r="C4" s="457"/>
-      <c r="D4" s="457"/>
-      <c r="E4" s="457"/>
-      <c r="F4" s="457"/>
+      <c r="B4" s="449"/>
+      <c r="C4" s="449"/>
+      <c r="D4" s="449"/>
+      <c r="E4" s="449"/>
+      <c r="F4" s="449"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="O4" s="3"/>
@@ -46543,32 +46531,32 @@
       <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="458" t="s">
+      <c r="C5" s="450" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="459"/>
-      <c r="E5" s="458" t="s">
+      <c r="D5" s="451"/>
+      <c r="E5" s="450" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="459"/>
-      <c r="G5" s="460" t="s">
+      <c r="F5" s="451"/>
+      <c r="G5" s="452" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="461"/>
-      <c r="I5" s="458" t="s">
+      <c r="H5" s="453"/>
+      <c r="I5" s="450" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="459"/>
-      <c r="K5" s="454" t="s">
+      <c r="J5" s="451"/>
+      <c r="K5" s="456" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="454" t="s">
+      <c r="L5" s="456" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="454" t="s">
+      <c r="M5" s="456" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="454" t="s">
+      <c r="N5" s="456" t="s">
         <v>6</v>
       </c>
       <c r="O5" s="283" t="s">
@@ -46579,26 +46567,26 @@
       <c r="B6" s="282" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="452" t="s">
+      <c r="C6" s="454" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="453"/>
-      <c r="E6" s="452" t="s">
+      <c r="D6" s="455"/>
+      <c r="E6" s="454" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="453"/>
-      <c r="G6" s="452" t="s">
+      <c r="F6" s="455"/>
+      <c r="G6" s="454" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="453"/>
-      <c r="I6" s="452" t="s">
+      <c r="H6" s="455"/>
+      <c r="I6" s="454" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="453"/>
-      <c r="K6" s="455"/>
-      <c r="L6" s="455"/>
-      <c r="M6" s="455"/>
-      <c r="N6" s="455"/>
+      <c r="J6" s="455"/>
+      <c r="K6" s="457"/>
+      <c r="L6" s="457"/>
+      <c r="M6" s="457"/>
+      <c r="N6" s="457"/>
       <c r="O6" s="284" t="s">
         <v>116</v>
       </c>
@@ -49167,12 +49155,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
@@ -49181,6 +49163,12 @@
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49236,137 +49224,137 @@
       <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:29" ht="26.25">
-      <c r="A2" s="470" t="s">
+      <c r="A2" s="458" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="471"/>
-      <c r="C2" s="471"/>
-      <c r="D2" s="471"/>
-      <c r="E2" s="472"/>
+      <c r="B2" s="459"/>
+      <c r="C2" s="459"/>
+      <c r="D2" s="459"/>
+      <c r="E2" s="460"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="470" t="s">
+      <c r="G2" s="458" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="471"/>
-      <c r="I2" s="471"/>
-      <c r="J2" s="471"/>
-      <c r="K2" s="472"/>
+      <c r="H2" s="459"/>
+      <c r="I2" s="459"/>
+      <c r="J2" s="459"/>
+      <c r="K2" s="460"/>
       <c r="L2" s="43"/>
-      <c r="M2" s="470" t="s">
+      <c r="M2" s="458" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="471"/>
-      <c r="O2" s="471"/>
-      <c r="P2" s="471"/>
-      <c r="Q2" s="472"/>
+      <c r="N2" s="459"/>
+      <c r="O2" s="459"/>
+      <c r="P2" s="459"/>
+      <c r="Q2" s="460"/>
       <c r="R2" s="43"/>
-      <c r="S2" s="470" t="s">
+      <c r="S2" s="458" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="471"/>
-      <c r="U2" s="471"/>
-      <c r="V2" s="471"/>
-      <c r="W2" s="472"/>
+      <c r="T2" s="459"/>
+      <c r="U2" s="459"/>
+      <c r="V2" s="459"/>
+      <c r="W2" s="460"/>
       <c r="X2" s="43"/>
-      <c r="Y2" s="470" t="s">
+      <c r="Y2" s="458" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="471"/>
-      <c r="AA2" s="471"/>
-      <c r="AB2" s="471"/>
-      <c r="AC2" s="472"/>
+      <c r="Z2" s="459"/>
+      <c r="AA2" s="459"/>
+      <c r="AB2" s="459"/>
+      <c r="AC2" s="460"/>
     </row>
     <row r="3" spans="1:29" ht="26.25">
-      <c r="A3" s="462" t="s">
+      <c r="A3" s="461" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="463"/>
-      <c r="C3" s="463"/>
-      <c r="D3" s="463"/>
-      <c r="E3" s="464"/>
+      <c r="B3" s="462"/>
+      <c r="C3" s="462"/>
+      <c r="D3" s="462"/>
+      <c r="E3" s="463"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="462" t="s">
+      <c r="G3" s="461" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="463"/>
-      <c r="I3" s="463"/>
-      <c r="J3" s="463"/>
-      <c r="K3" s="464"/>
+      <c r="H3" s="462"/>
+      <c r="I3" s="462"/>
+      <c r="J3" s="462"/>
+      <c r="K3" s="463"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="462" t="s">
+      <c r="M3" s="461" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="463"/>
-      <c r="O3" s="463"/>
-      <c r="P3" s="463"/>
-      <c r="Q3" s="464"/>
+      <c r="N3" s="462"/>
+      <c r="O3" s="462"/>
+      <c r="P3" s="462"/>
+      <c r="Q3" s="463"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="462" t="s">
+      <c r="S3" s="461" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="463"/>
-      <c r="U3" s="463"/>
-      <c r="V3" s="463"/>
-      <c r="W3" s="464"/>
+      <c r="T3" s="462"/>
+      <c r="U3" s="462"/>
+      <c r="V3" s="462"/>
+      <c r="W3" s="463"/>
       <c r="X3" s="4"/>
-      <c r="Y3" s="462" t="s">
+      <c r="Y3" s="461" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="463"/>
-      <c r="AA3" s="463"/>
-      <c r="AB3" s="463"/>
-      <c r="AC3" s="464"/>
+      <c r="Z3" s="462"/>
+      <c r="AA3" s="462"/>
+      <c r="AB3" s="462"/>
+      <c r="AC3" s="463"/>
     </row>
     <row r="4" spans="1:29" ht="26.25">
-      <c r="A4" s="465" t="s">
+      <c r="A4" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="466"/>
-      <c r="C4" s="467">
+      <c r="B4" s="465"/>
+      <c r="C4" s="466">
         <v>42337</v>
       </c>
-      <c r="D4" s="468"/>
-      <c r="E4" s="469"/>
+      <c r="D4" s="467"/>
+      <c r="E4" s="468"/>
       <c r="F4" s="43"/>
-      <c r="G4" s="465" t="s">
+      <c r="G4" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="466"/>
-      <c r="I4" s="467">
+      <c r="H4" s="465"/>
+      <c r="I4" s="466">
         <v>42503</v>
       </c>
-      <c r="J4" s="468"/>
-      <c r="K4" s="469"/>
+      <c r="J4" s="467"/>
+      <c r="K4" s="468"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="465" t="s">
+      <c r="M4" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="466"/>
-      <c r="O4" s="467">
+      <c r="N4" s="465"/>
+      <c r="O4" s="466">
         <v>42337</v>
       </c>
-      <c r="P4" s="468"/>
-      <c r="Q4" s="469"/>
+      <c r="P4" s="467"/>
+      <c r="Q4" s="468"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="465" t="s">
+      <c r="S4" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="466"/>
-      <c r="U4" s="467">
+      <c r="T4" s="465"/>
+      <c r="U4" s="466">
         <v>42502</v>
       </c>
-      <c r="V4" s="468"/>
-      <c r="W4" s="469"/>
+      <c r="V4" s="467"/>
+      <c r="W4" s="468"/>
       <c r="X4" s="4"/>
-      <c r="Y4" s="465" t="s">
+      <c r="Y4" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="Z4" s="466"/>
-      <c r="AA4" s="467">
+      <c r="Z4" s="465"/>
+      <c r="AA4" s="466">
         <v>42530</v>
       </c>
-      <c r="AB4" s="468"/>
-      <c r="AC4" s="469"/>
+      <c r="AB4" s="467"/>
+      <c r="AC4" s="468"/>
     </row>
     <row r="5" spans="1:29" ht="26.25">
       <c r="A5" s="46">
@@ -51474,6 +51462,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="M3:Q3"/>
     <mergeCell ref="M4:N4"/>
@@ -51486,14 +51482,6 @@
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="U4:W4"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>